<commit_message>
Fix filtering script that created duplicates in Continuous Cover file
</commit_message>
<xml_diff>
--- a/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
+++ b/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephen.wood/Box Sync/Work/The Nature Conservancy/Global Soils/AgEvidence/code-and-data/AgEvidence_Kenya/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E87990-1342-5848-9A81-0FBBB4C73480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6EE6B8-7246-4242-8E8F-948C0CD58729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="1380" windowWidth="16900" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="grouplists_Kenya_2021-07-14" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'grouplists_Kenya_2021-07-14'!$A$1:$J$210</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'grouplists_Kenya_2021-07-14'!$A$1:$J$209</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="201">
   <si>
     <t>Review</t>
   </si>
@@ -1493,11 +1493,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J210"/>
+  <dimension ref="A1:J209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F222" sqref="F222"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A94" sqref="A94:XFD94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4490,7 +4490,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B94" t="s">
         <v>24</v>
@@ -4522,16 +4522,16 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B95" t="s">
         <v>24</v>
       </c>
       <c r="C95" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D95" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="E95" t="s">
         <v>27</v>
@@ -4554,7 +4554,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B96" t="s">
         <v>24</v>
@@ -4563,7 +4563,7 @@
         <v>103</v>
       </c>
       <c r="D96" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="E96" t="s">
         <v>27</v>
@@ -4586,7 +4586,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B97" t="s">
         <v>24</v>
@@ -4595,7 +4595,7 @@
         <v>103</v>
       </c>
       <c r="D97" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E97" t="s">
         <v>27</v>
@@ -4604,21 +4604,21 @@
         <v>77</v>
       </c>
       <c r="G97" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H97" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I97" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J97" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B98" t="s">
         <v>24</v>
@@ -4627,7 +4627,7 @@
         <v>103</v>
       </c>
       <c r="D98" t="s">
-        <v>178</v>
+        <v>104</v>
       </c>
       <c r="E98" t="s">
         <v>27</v>
@@ -4636,21 +4636,21 @@
         <v>77</v>
       </c>
       <c r="G98" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H98" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I98" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J98" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B99" t="s">
         <v>24</v>
@@ -4659,13 +4659,13 @@
         <v>103</v>
       </c>
       <c r="D99" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E99" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F99" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G99" t="s">
         <v>14</v>
@@ -4682,7 +4682,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B100" t="s">
         <v>24</v>
@@ -4714,7 +4714,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B101" t="s">
         <v>24</v>
@@ -4723,7 +4723,7 @@
         <v>103</v>
       </c>
       <c r="D101" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E101" t="s">
         <v>22</v>
@@ -4746,7 +4746,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B102" t="s">
         <v>24</v>
@@ -4778,7 +4778,7 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B103" t="s">
         <v>24</v>
@@ -4787,13 +4787,13 @@
         <v>103</v>
       </c>
       <c r="D103" t="s">
-        <v>106</v>
+        <v>176</v>
       </c>
       <c r="E103" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F103" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G103" t="s">
         <v>14</v>
@@ -4810,7 +4810,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B104" t="s">
         <v>24</v>
@@ -4842,7 +4842,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B105" t="s">
         <v>24</v>
@@ -4851,7 +4851,7 @@
         <v>103</v>
       </c>
       <c r="D105" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="E105" t="s">
         <v>27</v>
@@ -4874,7 +4874,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B106" t="s">
         <v>24</v>
@@ -4912,16 +4912,16 @@
         <v>24</v>
       </c>
       <c r="C107" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="D107" t="s">
-        <v>189</v>
+        <v>108</v>
       </c>
       <c r="E107" t="s">
         <v>27</v>
       </c>
       <c r="F107" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G107" t="s">
         <v>14</v>
@@ -4938,7 +4938,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B108" t="s">
         <v>24</v>
@@ -4947,13 +4947,13 @@
         <v>25</v>
       </c>
       <c r="D108" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E108" t="s">
         <v>27</v>
       </c>
       <c r="F108" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G108" t="s">
         <v>14</v>
@@ -4970,7 +4970,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B109" t="s">
         <v>24</v>
@@ -5002,7 +5002,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B110" t="s">
         <v>24</v>
@@ -5011,30 +5011,30 @@
         <v>25</v>
       </c>
       <c r="D110" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E110" t="s">
         <v>27</v>
       </c>
       <c r="F110" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G110" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H110" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I110" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J110" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B111" t="s">
         <v>24</v>
@@ -5066,7 +5066,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B112" t="s">
         <v>24</v>
@@ -5098,34 +5098,34 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B113" t="s">
         <v>24</v>
       </c>
       <c r="C113" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
       <c r="D113" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E113" t="s">
         <v>27</v>
       </c>
       <c r="F113" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G113" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="H113" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="I113" t="s">
         <v>22</v>
       </c>
       <c r="J113" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
@@ -5139,30 +5139,30 @@
         <v>111</v>
       </c>
       <c r="D114" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E114" t="s">
         <v>27</v>
       </c>
       <c r="F114" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="G114" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H114" t="s">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="I114" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="J114" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B115" t="s">
         <v>24</v>
@@ -5171,13 +5171,13 @@
         <v>111</v>
       </c>
       <c r="D115" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E115" t="s">
         <v>27</v>
       </c>
       <c r="F115" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="G115" t="s">
         <v>14</v>
@@ -5194,7 +5194,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B116" t="s">
         <v>24</v>
@@ -5203,7 +5203,7 @@
         <v>111</v>
       </c>
       <c r="D116" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E116" t="s">
         <v>27</v>
@@ -5226,7 +5226,7 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B117" t="s">
         <v>24</v>
@@ -5235,13 +5235,13 @@
         <v>111</v>
       </c>
       <c r="D117" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E117" t="s">
         <v>27</v>
       </c>
       <c r="F117" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G117" t="s">
         <v>14</v>
@@ -5258,7 +5258,7 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B118" t="s">
         <v>24</v>
@@ -5296,13 +5296,13 @@
         <v>24</v>
       </c>
       <c r="C119" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D119" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E119" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F119" t="s">
         <v>26</v>
@@ -5322,7 +5322,7 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B120" t="s">
         <v>24</v>
@@ -5354,7 +5354,7 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B121" t="s">
         <v>24</v>
@@ -5363,7 +5363,7 @@
         <v>112</v>
       </c>
       <c r="D121" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E121" t="s">
         <v>22</v>
@@ -5386,7 +5386,7 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B122" t="s">
         <v>24</v>
@@ -5418,34 +5418,34 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B123" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C123" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="D123" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E123" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F123" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G123" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="H123" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I123" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J123" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
@@ -5459,7 +5459,7 @@
         <v>40</v>
       </c>
       <c r="D124" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E124" t="s">
         <v>15</v>
@@ -5491,7 +5491,7 @@
         <v>40</v>
       </c>
       <c r="D125" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E125" t="s">
         <v>15</v>
@@ -5523,7 +5523,7 @@
         <v>40</v>
       </c>
       <c r="D126" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E126" t="s">
         <v>15</v>
@@ -5555,7 +5555,7 @@
         <v>40</v>
       </c>
       <c r="D127" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E127" t="s">
         <v>15</v>
@@ -5578,7 +5578,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B128" t="s">
         <v>41</v>
@@ -5587,7 +5587,7 @@
         <v>40</v>
       </c>
       <c r="D128" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="E128" t="s">
         <v>15</v>
@@ -5610,16 +5610,16 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B129" t="s">
         <v>41</v>
       </c>
       <c r="C129" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D129" t="s">
-        <v>170</v>
+        <v>124</v>
       </c>
       <c r="E129" t="s">
         <v>15</v>
@@ -5628,16 +5628,16 @@
         <v>16</v>
       </c>
       <c r="G129" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H129" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="I129" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J129" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
@@ -5651,7 +5651,7 @@
         <v>42</v>
       </c>
       <c r="D130" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E130" t="s">
         <v>15</v>
@@ -5683,7 +5683,7 @@
         <v>42</v>
       </c>
       <c r="D131" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E131" t="s">
         <v>15</v>
@@ -5706,7 +5706,7 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B132" t="s">
         <v>41</v>
@@ -5715,7 +5715,7 @@
         <v>42</v>
       </c>
       <c r="D132" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E132" t="s">
         <v>15</v>
@@ -5738,7 +5738,7 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B133" t="s">
         <v>41</v>
@@ -5747,7 +5747,7 @@
         <v>42</v>
       </c>
       <c r="D133" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E133" t="s">
         <v>15</v>
@@ -5776,13 +5776,13 @@
         <v>41</v>
       </c>
       <c r="C134" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="D134" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E134" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F134" t="s">
         <v>16</v>
@@ -5802,7 +5802,7 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B135" t="s">
         <v>41</v>
@@ -5834,7 +5834,7 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B136" t="s">
         <v>41</v>
@@ -5843,25 +5843,25 @@
         <v>130</v>
       </c>
       <c r="D136" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E136" t="s">
         <v>27</v>
       </c>
       <c r="F136" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="G136" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H136" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="I136" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J136" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
@@ -5875,7 +5875,7 @@
         <v>130</v>
       </c>
       <c r="D137" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E137" t="s">
         <v>27</v>
@@ -5898,7 +5898,7 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B138" t="s">
         <v>41</v>
@@ -5930,7 +5930,7 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B139" t="s">
         <v>41</v>
@@ -5939,7 +5939,7 @@
         <v>130</v>
       </c>
       <c r="D139" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E139" t="s">
         <v>27</v>
@@ -5962,7 +5962,7 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B140" t="s">
         <v>41</v>
@@ -5994,7 +5994,7 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B141" t="s">
         <v>41</v>
@@ -6003,7 +6003,7 @@
         <v>130</v>
       </c>
       <c r="D141" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E141" t="s">
         <v>27</v>
@@ -6026,7 +6026,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B142" t="s">
         <v>41</v>
@@ -6058,7 +6058,7 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B143" t="s">
         <v>41</v>
@@ -6067,25 +6067,25 @@
         <v>130</v>
       </c>
       <c r="D143" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E143" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F143" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="G143" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H143" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="I143" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="J143" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
@@ -6096,16 +6096,16 @@
         <v>41</v>
       </c>
       <c r="C144" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D144" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E144" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F144" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="G144" t="s">
         <v>14</v>
@@ -6122,7 +6122,7 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B145" t="s">
         <v>41</v>
@@ -6152,88 +6152,88 @@
         <v>14</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
+    <row r="146" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C146" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D146" t="s">
-        <v>138</v>
-      </c>
-      <c r="E146" t="s">
+      <c r="D146" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E146" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F146" t="s">
+      <c r="F146" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G146" t="s">
-        <v>14</v>
-      </c>
-      <c r="H146" t="s">
-        <v>14</v>
-      </c>
-      <c r="I146" t="s">
-        <v>14</v>
-      </c>
-      <c r="J146" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B147" s="1" t="s">
+      <c r="G146" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H146" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I146" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J146" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>10</v>
+      </c>
+      <c r="B147" t="s">
         <v>41</v>
       </c>
-      <c r="C147" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F147" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G147" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H147" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I147" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J147" s="1" t="s">
-        <v>26</v>
+      <c r="C147" t="s">
+        <v>140</v>
+      </c>
+      <c r="D147" t="s">
+        <v>129</v>
+      </c>
+      <c r="E147" t="s">
+        <v>22</v>
+      </c>
+      <c r="F147" t="s">
+        <v>26</v>
+      </c>
+      <c r="G147" t="s">
+        <v>14</v>
+      </c>
+      <c r="H147" t="s">
+        <v>14</v>
+      </c>
+      <c r="I147" t="s">
+        <v>14</v>
+      </c>
+      <c r="J147" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B148" t="s">
         <v>41</v>
       </c>
       <c r="C148" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D148" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="E148" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F148" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G148" t="s">
         <v>14</v>
@@ -6259,7 +6259,7 @@
         <v>141</v>
       </c>
       <c r="D149" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E149" t="s">
         <v>15</v>
@@ -6282,7 +6282,7 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B150" t="s">
         <v>41</v>
@@ -6291,7 +6291,7 @@
         <v>141</v>
       </c>
       <c r="D150" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E150" t="s">
         <v>15</v>
@@ -6323,7 +6323,7 @@
         <v>141</v>
       </c>
       <c r="D151" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E151" t="s">
         <v>15</v>
@@ -6346,7 +6346,7 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B152" t="s">
         <v>41</v>
@@ -6355,13 +6355,13 @@
         <v>141</v>
       </c>
       <c r="D152" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E152" t="s">
         <v>15</v>
       </c>
       <c r="F152" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="G152" t="s">
         <v>14</v>
@@ -6381,19 +6381,19 @@
         <v>17</v>
       </c>
       <c r="B153" t="s">
-        <v>41</v>
+        <v>147</v>
       </c>
       <c r="C153" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D153" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="E153" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F153" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G153" t="s">
         <v>14</v>
@@ -6410,7 +6410,7 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B154" t="s">
         <v>147</v>
@@ -6442,7 +6442,7 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B155" t="s">
         <v>147</v>
@@ -6451,7 +6451,7 @@
         <v>149</v>
       </c>
       <c r="D155" t="s">
-        <v>107</v>
+        <v>150</v>
       </c>
       <c r="E155" t="s">
         <v>22</v>
@@ -6474,7 +6474,7 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B156" t="s">
         <v>147</v>
@@ -6506,7 +6506,7 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B157" t="s">
         <v>147</v>
@@ -6515,7 +6515,7 @@
         <v>149</v>
       </c>
       <c r="D157" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E157" t="s">
         <v>22</v>
@@ -6538,7 +6538,7 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B158" t="s">
         <v>147</v>
@@ -6570,22 +6570,22 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B159" t="s">
         <v>147</v>
       </c>
       <c r="C159" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D159" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E159" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F159" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G159" t="s">
         <v>14</v>
@@ -6602,7 +6602,7 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B160" t="s">
         <v>147</v>
@@ -6634,7 +6634,7 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B161" t="s">
         <v>147</v>
@@ -6643,7 +6643,7 @@
         <v>153</v>
       </c>
       <c r="D161" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E161" t="s">
         <v>27</v>
@@ -6666,7 +6666,7 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B162" t="s">
         <v>147</v>
@@ -6698,7 +6698,7 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B163" t="s">
         <v>147</v>
@@ -6707,7 +6707,7 @@
         <v>153</v>
       </c>
       <c r="D163" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E163" t="s">
         <v>27</v>
@@ -6730,7 +6730,7 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B164" t="s">
         <v>147</v>
@@ -6762,7 +6762,7 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B165" t="s">
         <v>147</v>
@@ -6771,13 +6771,13 @@
         <v>153</v>
       </c>
       <c r="D165" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E165" t="s">
         <v>27</v>
       </c>
       <c r="F165" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="G165" t="s">
         <v>14</v>
@@ -6803,13 +6803,13 @@
         <v>153</v>
       </c>
       <c r="D166" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E166" t="s">
         <v>27</v>
       </c>
       <c r="F166" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="G166" t="s">
         <v>14</v>
@@ -6826,7 +6826,7 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B167" t="s">
         <v>147</v>
@@ -6858,7 +6858,7 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B168" t="s">
         <v>147</v>
@@ -6890,16 +6890,16 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B169" t="s">
         <v>147</v>
       </c>
       <c r="C169" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D169" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E169" t="s">
         <v>27</v>
@@ -6922,7 +6922,7 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B170" t="s">
         <v>147</v>
@@ -6954,7 +6954,7 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B171" t="s">
         <v>147</v>
@@ -6986,7 +6986,7 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B172" t="s">
         <v>147</v>
@@ -6995,13 +6995,13 @@
         <v>157</v>
       </c>
       <c r="D172" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E172" t="s">
         <v>27</v>
       </c>
       <c r="F172" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="G172" t="s">
         <v>14</v>
@@ -7027,13 +7027,13 @@
         <v>157</v>
       </c>
       <c r="D173" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E173" t="s">
         <v>27</v>
       </c>
       <c r="F173" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G173" t="s">
         <v>14</v>
@@ -7050,7 +7050,7 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B174" t="s">
         <v>147</v>
@@ -7065,7 +7065,7 @@
         <v>27</v>
       </c>
       <c r="F174" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G174" t="s">
         <v>14</v>
@@ -7082,7 +7082,7 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B175" t="s">
         <v>147</v>
@@ -7097,7 +7097,7 @@
         <v>27</v>
       </c>
       <c r="F175" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G175" t="s">
         <v>14</v>
@@ -7114,7 +7114,7 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B176" t="s">
         <v>147</v>
@@ -7123,13 +7123,13 @@
         <v>157</v>
       </c>
       <c r="D176" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E176" t="s">
         <v>27</v>
       </c>
       <c r="F176" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G176" t="s">
         <v>14</v>
@@ -7149,16 +7149,16 @@
         <v>10</v>
       </c>
       <c r="B177" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="C177" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D177" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E177" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F177" t="s">
         <v>16</v>
@@ -7178,7 +7178,7 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B178" t="s">
         <v>162</v>
@@ -7187,7 +7187,7 @@
         <v>163</v>
       </c>
       <c r="D178" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E178" t="s">
         <v>15</v>
@@ -7210,7 +7210,7 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B179" t="s">
         <v>162</v>
@@ -7242,7 +7242,7 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B180" t="s">
         <v>162</v>
@@ -7274,16 +7274,16 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B181" t="s">
         <v>162</v>
       </c>
       <c r="C181" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D181" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="E181" t="s">
         <v>15</v>
@@ -7306,7 +7306,7 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B182" t="s">
         <v>162</v>
@@ -7338,7 +7338,7 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B183" t="s">
         <v>162</v>
@@ -7347,7 +7347,7 @@
         <v>166</v>
       </c>
       <c r="D183" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E183" t="s">
         <v>15</v>
@@ -7379,7 +7379,7 @@
         <v>166</v>
       </c>
       <c r="D184" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E184" t="s">
         <v>15</v>
@@ -7408,10 +7408,10 @@
         <v>162</v>
       </c>
       <c r="C185" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D185" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E185" t="s">
         <v>15</v>
@@ -7434,22 +7434,22 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B186" t="s">
-        <v>162</v>
+        <v>37</v>
       </c>
       <c r="C186" t="s">
-        <v>167</v>
+        <v>45</v>
       </c>
       <c r="D186" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="E186" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F186" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G186" t="s">
         <v>14</v>
@@ -7472,10 +7472,10 @@
         <v>37</v>
       </c>
       <c r="C187" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="D187" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E187" t="s">
         <v>22</v>
@@ -7507,7 +7507,7 @@
         <v>78</v>
       </c>
       <c r="D188" t="s">
-        <v>175</v>
+        <v>83</v>
       </c>
       <c r="E188" t="s">
         <v>22</v>
@@ -7539,7 +7539,7 @@
         <v>78</v>
       </c>
       <c r="D189" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E189" t="s">
         <v>22</v>
@@ -7562,16 +7562,16 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B190" t="s">
         <v>37</v>
       </c>
       <c r="C190" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="D190" t="s">
-        <v>84</v>
+        <v>180</v>
       </c>
       <c r="E190" t="s">
         <v>22</v>
@@ -7603,7 +7603,7 @@
         <v>45</v>
       </c>
       <c r="D191" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E191" t="s">
         <v>22</v>
@@ -7632,10 +7632,10 @@
         <v>37</v>
       </c>
       <c r="C192" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="D192" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E192" t="s">
         <v>22</v>
@@ -7667,13 +7667,13 @@
         <v>78</v>
       </c>
       <c r="D193" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="E193" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F193" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G193" t="s">
         <v>14</v>
@@ -7699,7 +7699,7 @@
         <v>78</v>
       </c>
       <c r="D194" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E194" t="s">
         <v>27</v>
@@ -7728,16 +7728,16 @@
         <v>37</v>
       </c>
       <c r="C195" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="D195" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="E195" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F195" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G195" t="s">
         <v>14</v>
@@ -7757,31 +7757,31 @@
         <v>173</v>
       </c>
       <c r="B196" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="C196" t="s">
-        <v>89</v>
+        <v>183</v>
       </c>
       <c r="D196" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="E196" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F196" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G196" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H196" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="I196" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J196" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.2">
@@ -7792,10 +7792,10 @@
         <v>91</v>
       </c>
       <c r="C197" t="s">
-        <v>183</v>
+        <v>92</v>
       </c>
       <c r="D197" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E197" t="s">
         <v>15</v>
@@ -7804,16 +7804,16 @@
         <v>16</v>
       </c>
       <c r="G197" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H197" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="I197" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J197" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.2">
@@ -7827,13 +7827,13 @@
         <v>92</v>
       </c>
       <c r="D198" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E198" t="s">
         <v>15</v>
       </c>
       <c r="F198" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G198" t="s">
         <v>14</v>
@@ -7859,7 +7859,7 @@
         <v>92</v>
       </c>
       <c r="D199" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E199" t="s">
         <v>15</v>
@@ -7885,31 +7885,31 @@
         <v>173</v>
       </c>
       <c r="B200" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="C200" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="D200" t="s">
-        <v>187</v>
+        <v>23</v>
       </c>
       <c r="E200" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F200" t="s">
         <v>26</v>
       </c>
       <c r="G200" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H200" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I200" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J200" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.2">
@@ -7917,13 +7917,13 @@
         <v>173</v>
       </c>
       <c r="B201" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C201" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="D201" t="s">
-        <v>23</v>
+        <v>193</v>
       </c>
       <c r="E201" t="s">
         <v>27</v>
@@ -7932,16 +7932,16 @@
         <v>26</v>
       </c>
       <c r="G201" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="H201" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="I201" t="s">
         <v>22</v>
       </c>
       <c r="J201" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.2">
@@ -7955,7 +7955,7 @@
         <v>130</v>
       </c>
       <c r="D202" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E202" t="s">
         <v>27</v>
@@ -7987,13 +7987,13 @@
         <v>130</v>
       </c>
       <c r="D203" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E203" t="s">
         <v>27</v>
       </c>
       <c r="F203" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G203" t="s">
         <v>24</v>
@@ -8019,7 +8019,7 @@
         <v>130</v>
       </c>
       <c r="D204" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E204" t="s">
         <v>27</v>
@@ -8042,16 +8042,16 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B205" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C205" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="D205" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E205" t="s">
         <v>27</v>
@@ -8060,16 +8060,16 @@
         <v>77</v>
       </c>
       <c r="G205" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H205" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="I205" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="J205" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.2">
@@ -8083,7 +8083,7 @@
         <v>99</v>
       </c>
       <c r="D206" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E206" t="s">
         <v>27</v>
@@ -8106,16 +8106,16 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B207" t="s">
         <v>24</v>
       </c>
       <c r="C207" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D207" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E207" t="s">
         <v>27</v>
@@ -8144,16 +8144,16 @@
         <v>24</v>
       </c>
       <c r="C208" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="D208" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E208" t="s">
         <v>27</v>
       </c>
       <c r="F208" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G208" t="s">
         <v>14</v>
@@ -8179,7 +8179,7 @@
         <v>25</v>
       </c>
       <c r="D209" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E209" t="s">
         <v>27</v>
@@ -8188,58 +8188,26 @@
         <v>26</v>
       </c>
       <c r="G209" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H209" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I209" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J209" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A210" t="s">
-        <v>173</v>
-      </c>
-      <c r="B210" t="s">
-        <v>24</v>
-      </c>
-      <c r="C210" t="s">
-        <v>25</v>
-      </c>
-      <c r="D210" t="s">
-        <v>200</v>
-      </c>
-      <c r="E210" t="s">
-        <v>27</v>
-      </c>
-      <c r="F210" t="s">
-        <v>26</v>
-      </c>
-      <c r="G210" t="s">
-        <v>11</v>
-      </c>
-      <c r="H210" t="s">
-        <v>20</v>
-      </c>
-      <c r="I210" t="s">
-        <v>22</v>
-      </c>
-      <c r="J210" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J210" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J186">
+  <autoFilter ref="A1:J209" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J185">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:J235">
-    <sortCondition ref="D2:D235"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:J234">
+    <sortCondition ref="D2:D234"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
matched grouping names to data files groupings to resolve NAs
</commit_message>
<xml_diff>
--- a/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
+++ b/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesley.atwood\Desktop\GitHub\AgEvidence\AgEvidence_Kenya\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AE2D46-D9B2-4882-857A-128400B9B2D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980A5907-02A3-4CB1-A83A-BF9EAF074EE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28875" yWindow="0" windowWidth="23640" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29340" yWindow="1125" windowWidth="23640" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grouplists_Kenya_2021-07-14" sheetId="1" r:id="rId1"/>
@@ -567,9 +567,6 @@
     <t>Nitrogen Decomposition Rate Of Buried Residues</t>
   </si>
   <si>
-    <t>Carbon Decomposition Rate On Buried Residues</t>
-  </si>
-  <si>
     <t>Respiration</t>
   </si>
   <si>
@@ -637,6 +634,9 @@
   </si>
   <si>
     <t>Mineral-Associated Carbon</t>
+  </si>
+  <si>
+    <t>Phosphorus Decomposition Rate Of Buried Residues</t>
   </si>
 </sst>
 </file>
@@ -1497,16 +1497,16 @@
   <dimension ref="A1:J209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I196" sqref="I196"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" customWidth="1"/>
-    <col min="4" max="4" width="47.6328125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6328125" customWidth="1"/>
+    <col min="4" max="4" width="47.6328125" customWidth="1"/>
     <col min="5" max="6" width="25.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.36328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
@@ -2356,7 +2356,7 @@
         <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E27" t="s">
         <v>22</v>
@@ -3348,7 +3348,7 @@
         <v>45</v>
       </c>
       <c r="D58" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E58" t="s">
         <v>22</v>
@@ -4084,7 +4084,7 @@
         <v>78</v>
       </c>
       <c r="D81" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E81" t="s">
         <v>22</v>
@@ -4148,7 +4148,7 @@
         <v>78</v>
       </c>
       <c r="D83" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E83" t="s">
         <v>22</v>
@@ -4628,7 +4628,7 @@
         <v>99</v>
       </c>
       <c r="D98" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E98" t="s">
         <v>27</v>
@@ -4692,7 +4692,7 @@
         <v>89</v>
       </c>
       <c r="D100" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E100" t="s">
         <v>22</v>
@@ -4753,10 +4753,10 @@
         <v>91</v>
       </c>
       <c r="C102" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D102" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E102" t="s">
         <v>15</v>
@@ -4788,7 +4788,7 @@
         <v>103</v>
       </c>
       <c r="D103" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="E103" t="s">
         <v>27</v>
@@ -4852,7 +4852,7 @@
         <v>103</v>
       </c>
       <c r="D105" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E105" t="s">
         <v>27</v>
@@ -4916,7 +4916,7 @@
         <v>92</v>
       </c>
       <c r="D107" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E107" t="s">
         <v>15</v>
@@ -4980,7 +4980,7 @@
         <v>92</v>
       </c>
       <c r="D109" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E109" t="s">
         <v>15</v>
@@ -5012,7 +5012,7 @@
         <v>99</v>
       </c>
       <c r="D110" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E110" t="s">
         <v>27</v>
@@ -5076,7 +5076,7 @@
         <v>92</v>
       </c>
       <c r="D112" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E112" t="s">
         <v>15</v>
@@ -5140,7 +5140,7 @@
         <v>103</v>
       </c>
       <c r="D114" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E114" t="s">
         <v>27</v>
@@ -5332,7 +5332,7 @@
         <v>99</v>
       </c>
       <c r="D120" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E120" t="s">
         <v>27</v>
@@ -5396,7 +5396,7 @@
         <v>103</v>
       </c>
       <c r="D122" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E122" t="s">
         <v>27</v>
@@ -5972,7 +5972,7 @@
         <v>103</v>
       </c>
       <c r="D140" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="E140" t="s">
         <v>27</v>
@@ -6036,7 +6036,7 @@
         <v>103</v>
       </c>
       <c r="D142" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E142" t="s">
         <v>27</v>
@@ -6676,7 +6676,7 @@
         <v>25</v>
       </c>
       <c r="D162" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E162" t="s">
         <v>27</v>
@@ -6740,7 +6740,7 @@
         <v>25</v>
       </c>
       <c r="D164" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E164" t="s">
         <v>27</v>
@@ -7668,7 +7668,7 @@
         <v>130</v>
       </c>
       <c r="D193" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E193" t="s">
         <v>27</v>
@@ -7700,7 +7700,7 @@
         <v>130</v>
       </c>
       <c r="D194" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E194" t="s">
         <v>27</v>
@@ -7732,7 +7732,7 @@
         <v>130</v>
       </c>
       <c r="D195" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E195" t="s">
         <v>27</v>
@@ -7764,7 +7764,7 @@
         <v>130</v>
       </c>
       <c r="D196" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E196" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
grouping and normative effects updated
</commit_message>
<xml_diff>
--- a/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
+++ b/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesley.atwood\Desktop\GitHub\AgEvidence\AgEvidence_Kenya\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4571023-F7E7-428D-A0D5-888EFC5CC783}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0A936D-E84C-469A-AAB3-DDCECD1641F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40935" yWindow="0" windowWidth="14745" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29490" yWindow="2415" windowWidth="28425" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grouplists_Kenya_2021-07-14" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'grouplists_Kenya_2021-07-14'!$A$1:$J$209</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'grouplists_Kenya_2021-07-14'!$A$1:$J$211</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2110" uniqueCount="203">
   <si>
     <t>Review</t>
   </si>
@@ -637,6 +637,12 @@
   </si>
   <si>
     <t>Phosphorus Decomposition Rate Of Buried Residues</t>
+  </si>
+  <si>
+    <t>Misc. Micro-nutrients</t>
+  </si>
+  <si>
+    <t>Variable Cost</t>
   </si>
 </sst>
 </file>
@@ -1133,10 +1139,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1493,11 +1500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J209"/>
+  <dimension ref="A1:J211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C213" sqref="C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4616,85 +4623,85 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+    <row r="98" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C98" t="s">
+        <v>95</v>
+      </c>
+      <c r="D98" t="s">
+        <v>97</v>
+      </c>
+      <c r="E98" t="s">
+        <v>22</v>
+      </c>
+      <c r="F98" t="s">
+        <v>26</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D98" t="s">
-        <v>185</v>
-      </c>
-      <c r="E98" t="s">
+      <c r="D99" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F98" t="s">
-        <v>26</v>
-      </c>
-      <c r="G98" t="s">
-        <v>14</v>
-      </c>
-      <c r="H98" t="s">
-        <v>14</v>
-      </c>
-      <c r="I98" t="s">
-        <v>14</v>
-      </c>
-      <c r="J98" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
-        <v>173</v>
-      </c>
-      <c r="B99" t="s">
-        <v>91</v>
-      </c>
-      <c r="C99" t="s">
-        <v>92</v>
-      </c>
-      <c r="D99" t="s">
-        <v>186</v>
-      </c>
-      <c r="E99" t="s">
-        <v>15</v>
-      </c>
-      <c r="F99" t="s">
-        <v>26</v>
-      </c>
-      <c r="G99" t="s">
-        <v>14</v>
-      </c>
-      <c r="H99" t="s">
-        <v>14</v>
-      </c>
-      <c r="I99" t="s">
-        <v>14</v>
-      </c>
-      <c r="J99" t="s">
+      <c r="F99" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H99" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J99" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B100" t="s">
         <v>91</v>
       </c>
       <c r="C100" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D100" t="s">
-        <v>96</v>
+        <v>185</v>
       </c>
       <c r="E100" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F100" t="s">
         <v>26</v>
@@ -4714,19 +4721,19 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B101" t="s">
         <v>91</v>
       </c>
       <c r="C101" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D101" t="s">
-        <v>97</v>
+        <v>186</v>
       </c>
       <c r="E101" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F101" t="s">
         <v>26</v>
@@ -4746,22 +4753,22 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B102" t="s">
         <v>91</v>
       </c>
       <c r="C102" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D102" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E102" t="s">
         <v>22</v>
       </c>
       <c r="F102" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G102" t="s">
         <v>14</v>
@@ -4778,22 +4785,22 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B103" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="C103" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D103" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E103" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F103" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G103" t="s">
         <v>14</v>
@@ -4813,16 +4820,16 @@
         <v>10</v>
       </c>
       <c r="B104" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="C104" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D104" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E104" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F104" t="s">
         <v>77</v>
@@ -4851,7 +4858,7 @@
         <v>99</v>
       </c>
       <c r="D105" t="s">
-        <v>194</v>
+        <v>101</v>
       </c>
       <c r="E105" t="s">
         <v>27</v>
@@ -4874,7 +4881,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B106" t="s">
         <v>24</v>
@@ -4883,7 +4890,7 @@
         <v>99</v>
       </c>
       <c r="D106" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E106" t="s">
         <v>27</v>
@@ -4906,7 +4913,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B107" t="s">
         <v>24</v>
@@ -4915,7 +4922,7 @@
         <v>99</v>
       </c>
       <c r="D107" t="s">
-        <v>102</v>
+        <v>194</v>
       </c>
       <c r="E107" t="s">
         <v>27</v>
@@ -4938,7 +4945,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B108" t="s">
         <v>24</v>
@@ -4947,7 +4954,7 @@
         <v>99</v>
       </c>
       <c r="D108" t="s">
-        <v>195</v>
+        <v>100</v>
       </c>
       <c r="E108" t="s">
         <v>27</v>
@@ -4970,7 +4977,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B109" t="s">
         <v>24</v>
@@ -5002,7 +5009,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B110" t="s">
         <v>24</v>
@@ -5011,7 +5018,7 @@
         <v>99</v>
       </c>
       <c r="D110" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E110" t="s">
         <v>27</v>
@@ -5034,16 +5041,16 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B111" t="s">
         <v>24</v>
       </c>
       <c r="C111" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D111" t="s">
-        <v>187</v>
+        <v>102</v>
       </c>
       <c r="E111" t="s">
         <v>27</v>
@@ -5066,16 +5073,16 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B112" t="s">
         <v>24</v>
       </c>
       <c r="C112" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D112" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="E112" t="s">
         <v>27</v>
@@ -5084,16 +5091,16 @@
         <v>77</v>
       </c>
       <c r="G112" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H112" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I112" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J112" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.35">
@@ -5107,13 +5114,13 @@
         <v>103</v>
       </c>
       <c r="D113" t="s">
-        <v>105</v>
+        <v>187</v>
       </c>
       <c r="E113" t="s">
         <v>27</v>
       </c>
       <c r="F113" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G113" t="s">
         <v>14</v>
@@ -5139,25 +5146,25 @@
         <v>103</v>
       </c>
       <c r="D114" t="s">
-        <v>106</v>
+        <v>177</v>
       </c>
       <c r="E114" t="s">
         <v>27</v>
       </c>
       <c r="F114" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G114" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H114" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I114" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J114" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.35">
@@ -5171,13 +5178,13 @@
         <v>103</v>
       </c>
       <c r="D115" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
       <c r="E115" t="s">
         <v>27</v>
       </c>
       <c r="F115" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G115" t="s">
         <v>14</v>
@@ -5203,13 +5210,13 @@
         <v>103</v>
       </c>
       <c r="D116" t="s">
-        <v>188</v>
+        <v>106</v>
       </c>
       <c r="E116" t="s">
         <v>27</v>
       </c>
       <c r="F116" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G116" t="s">
         <v>14</v>
@@ -5226,7 +5233,7 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B117" t="s">
         <v>24</v>
@@ -5235,7 +5242,7 @@
         <v>103</v>
       </c>
       <c r="D117" t="s">
-        <v>104</v>
+        <v>176</v>
       </c>
       <c r="E117" t="s">
         <v>27</v>
@@ -5258,7 +5265,7 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B118" t="s">
         <v>24</v>
@@ -5267,7 +5274,7 @@
         <v>103</v>
       </c>
       <c r="D118" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E118" t="s">
         <v>27</v>
@@ -5290,7 +5297,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B119" t="s">
         <v>24</v>
@@ -5299,13 +5306,13 @@
         <v>103</v>
       </c>
       <c r="D119" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E119" t="s">
         <v>27</v>
       </c>
       <c r="F119" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G119" t="s">
         <v>14</v>
@@ -5331,13 +5338,13 @@
         <v>103</v>
       </c>
       <c r="D120" t="s">
-        <v>106</v>
+        <v>187</v>
       </c>
       <c r="E120" t="s">
         <v>27</v>
       </c>
       <c r="F120" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G120" t="s">
         <v>14</v>
@@ -5363,13 +5370,13 @@
         <v>103</v>
       </c>
       <c r="D121" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
       <c r="E121" t="s">
         <v>27</v>
       </c>
       <c r="F121" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G121" t="s">
         <v>14</v>
@@ -5395,13 +5402,13 @@
         <v>103</v>
       </c>
       <c r="D122" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="E122" t="s">
         <v>27</v>
       </c>
       <c r="F122" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G122" t="s">
         <v>14</v>
@@ -5427,7 +5434,7 @@
         <v>103</v>
       </c>
       <c r="D123" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="E123" t="s">
         <v>27</v>
@@ -5450,48 +5457,48 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B124" t="s">
         <v>24</v>
       </c>
       <c r="C124" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="D124" t="s">
-        <v>110</v>
+        <v>200</v>
       </c>
       <c r="E124" t="s">
         <v>27</v>
       </c>
       <c r="F124" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G124" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H124" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I124" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="J124" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B125" t="s">
         <v>24</v>
       </c>
       <c r="C125" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="D125" t="s">
-        <v>109</v>
+        <v>197</v>
       </c>
       <c r="E125" t="s">
         <v>27</v>
@@ -5514,7 +5521,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B126" t="s">
         <v>24</v>
@@ -5546,7 +5553,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B127" t="s">
         <v>24</v>
@@ -5555,13 +5562,13 @@
         <v>25</v>
       </c>
       <c r="D127" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E127" t="s">
         <v>27</v>
       </c>
       <c r="F127" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G127" t="s">
         <v>14</v>
@@ -5578,7 +5585,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B128" t="s">
         <v>24</v>
@@ -5587,25 +5594,25 @@
         <v>25</v>
       </c>
       <c r="D128" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E128" t="s">
         <v>27</v>
       </c>
       <c r="F128" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G128" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H128" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I128" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J128" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.35">
@@ -5619,7 +5626,7 @@
         <v>25</v>
       </c>
       <c r="D129" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E129" t="s">
         <v>27</v>
@@ -5628,16 +5635,16 @@
         <v>26</v>
       </c>
       <c r="G129" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H129" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I129" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="J129" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.35">
@@ -5651,25 +5658,25 @@
         <v>25</v>
       </c>
       <c r="D130" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="E130" t="s">
         <v>27</v>
       </c>
       <c r="F130" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G130" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H130" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I130" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="J130" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.35">
@@ -5683,7 +5690,7 @@
         <v>25</v>
       </c>
       <c r="D131" t="s">
-        <v>198</v>
+        <v>110</v>
       </c>
       <c r="E131" t="s">
         <v>27</v>
@@ -5692,16 +5699,16 @@
         <v>26</v>
       </c>
       <c r="G131" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H131" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I131" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J131" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.35">
@@ -5715,7 +5722,7 @@
         <v>25</v>
       </c>
       <c r="D132" t="s">
-        <v>199</v>
+        <v>23</v>
       </c>
       <c r="E132" t="s">
         <v>27</v>
@@ -5738,71 +5745,71 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B133" t="s">
         <v>24</v>
       </c>
       <c r="C133" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="D133" t="s">
-        <v>115</v>
+        <v>198</v>
       </c>
       <c r="E133" t="s">
         <v>27</v>
       </c>
       <c r="F133" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G133" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H133" t="s">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="I133" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="J133" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B134" t="s">
         <v>24</v>
       </c>
       <c r="C134" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="D134" t="s">
-        <v>114</v>
+        <v>199</v>
       </c>
       <c r="E134" t="s">
         <v>27</v>
       </c>
       <c r="F134" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G134" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H134" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I134" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J134" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B135" t="s">
         <v>24</v>
@@ -5811,30 +5818,30 @@
         <v>111</v>
       </c>
       <c r="D135" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E135" t="s">
         <v>27</v>
       </c>
       <c r="F135" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G135" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H135" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="I135" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J135" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B136" t="s">
         <v>24</v>
@@ -5843,13 +5850,13 @@
         <v>111</v>
       </c>
       <c r="D136" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E136" t="s">
         <v>27</v>
       </c>
       <c r="F136" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="G136" t="s">
         <v>14</v>
@@ -5866,7 +5873,7 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B137" t="s">
         <v>24</v>
@@ -5898,7 +5905,7 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B138" t="s">
         <v>24</v>
@@ -5907,13 +5914,13 @@
         <v>111</v>
       </c>
       <c r="D138" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E138" t="s">
         <v>27</v>
       </c>
       <c r="F138" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="G138" t="s">
         <v>14</v>
@@ -5936,13 +5943,13 @@
         <v>24</v>
       </c>
       <c r="C139" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D139" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E139" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F139" t="s">
         <v>26</v>
@@ -5962,22 +5969,22 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B140" t="s">
         <v>24</v>
       </c>
       <c r="C140" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D140" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E140" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F140" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G140" t="s">
         <v>14</v>
@@ -5994,7 +6001,7 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B141" t="s">
         <v>24</v>
@@ -6026,7 +6033,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B142" t="s">
         <v>24</v>
@@ -6058,66 +6065,66 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B143" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C143" t="s">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D143" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E143" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F143" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G143" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H143" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="I143" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J143" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B144" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C144" t="s">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D144" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E144" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F144" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G144" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H144" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="I144" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J144" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.35">
@@ -6131,7 +6138,7 @@
         <v>40</v>
       </c>
       <c r="D145" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E145" t="s">
         <v>15</v>
@@ -6152,7 +6159,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="146" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>10</v>
       </c>
@@ -6163,7 +6170,7 @@
         <v>40</v>
       </c>
       <c r="D146" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E146" t="s">
         <v>15</v>
@@ -6195,7 +6202,7 @@
         <v>40</v>
       </c>
       <c r="D147" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E147" t="s">
         <v>15</v>
@@ -6216,9 +6223,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B148" t="s">
         <v>41</v>
@@ -6227,7 +6234,7 @@
         <v>40</v>
       </c>
       <c r="D148" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="E148" t="s">
         <v>15</v>
@@ -6256,10 +6263,10 @@
         <v>41</v>
       </c>
       <c r="C149" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D149" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E149" t="s">
         <v>15</v>
@@ -6268,30 +6275,30 @@
         <v>16</v>
       </c>
       <c r="G149" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="H149" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I149" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J149" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B150" t="s">
         <v>41</v>
       </c>
       <c r="C150" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D150" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
       <c r="E150" t="s">
         <v>15</v>
@@ -6300,16 +6307,16 @@
         <v>16</v>
       </c>
       <c r="G150" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="H150" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I150" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J150" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.35">
@@ -6323,7 +6330,7 @@
         <v>42</v>
       </c>
       <c r="D151" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E151" t="s">
         <v>15</v>
@@ -6355,7 +6362,7 @@
         <v>42</v>
       </c>
       <c r="D152" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E152" t="s">
         <v>15</v>
@@ -6378,7 +6385,7 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B153" t="s">
         <v>41</v>
@@ -6387,7 +6394,7 @@
         <v>42</v>
       </c>
       <c r="D153" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E153" t="s">
         <v>15</v>
@@ -6416,13 +6423,13 @@
         <v>41</v>
       </c>
       <c r="C154" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
       <c r="D154" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E154" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F154" t="s">
         <v>16</v>
@@ -6442,34 +6449,34 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B155" t="s">
         <v>41</v>
       </c>
       <c r="C155" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
       <c r="D155" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E155" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F155" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="G155" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H155" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="I155" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="J155" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.35">
@@ -6483,25 +6490,25 @@
         <v>130</v>
       </c>
       <c r="D156" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E156" t="s">
         <v>27</v>
       </c>
       <c r="F156" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="G156" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H156" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="I156" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="J156" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.35">
@@ -6515,7 +6522,7 @@
         <v>130</v>
       </c>
       <c r="D157" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E157" t="s">
         <v>27</v>
@@ -6547,7 +6554,7 @@
         <v>130</v>
       </c>
       <c r="D158" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E158" t="s">
         <v>27</v>
@@ -6579,30 +6586,30 @@
         <v>130</v>
       </c>
       <c r="D159" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E159" t="s">
         <v>27</v>
       </c>
       <c r="F159" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="G159" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H159" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="I159" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="J159" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B160" t="s">
         <v>41</v>
@@ -6611,30 +6618,30 @@
         <v>130</v>
       </c>
       <c r="D160" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E160" t="s">
         <v>27</v>
       </c>
       <c r="F160" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="G160" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H160" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="I160" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="J160" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B161" t="s">
         <v>41</v>
@@ -6643,25 +6650,25 @@
         <v>130</v>
       </c>
       <c r="D161" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E161" t="s">
         <v>27</v>
       </c>
       <c r="F161" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="G161" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H161" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="I161" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="J161" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.35">
@@ -6675,25 +6682,25 @@
         <v>130</v>
       </c>
       <c r="D162" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E162" t="s">
         <v>27</v>
       </c>
       <c r="F162" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="G162" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H162" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="I162" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="J162" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.35">
@@ -6707,7 +6714,7 @@
         <v>130</v>
       </c>
       <c r="D163" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E163" t="s">
         <v>27</v>
@@ -6739,13 +6746,13 @@
         <v>130</v>
       </c>
       <c r="D164" t="s">
-        <v>192</v>
+        <v>134</v>
       </c>
       <c r="E164" t="s">
         <v>27</v>
       </c>
       <c r="F164" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G164" t="s">
         <v>24</v>
@@ -6771,13 +6778,13 @@
         <v>130</v>
       </c>
       <c r="D165" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="E165" t="s">
         <v>27</v>
       </c>
       <c r="F165" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G165" t="s">
         <v>24</v>
@@ -6803,13 +6810,13 @@
         <v>130</v>
       </c>
       <c r="D166" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E166" t="s">
         <v>27</v>
       </c>
       <c r="F166" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G166" t="s">
         <v>24</v>
@@ -6835,13 +6842,13 @@
         <v>130</v>
       </c>
       <c r="D167" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E167" t="s">
         <v>27</v>
       </c>
       <c r="F167" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G167" t="s">
         <v>24</v>
@@ -6858,16 +6865,16 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B168" t="s">
         <v>41</v>
       </c>
       <c r="C168" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D168" t="s">
-        <v>138</v>
+        <v>190</v>
       </c>
       <c r="E168" t="s">
         <v>27</v>
@@ -6876,30 +6883,30 @@
         <v>77</v>
       </c>
       <c r="G168" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H168" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="I168" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="J168" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B169" t="s">
         <v>41</v>
       </c>
       <c r="C169" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D169" t="s">
-        <v>138</v>
+        <v>191</v>
       </c>
       <c r="E169" t="s">
         <v>27</v>
@@ -6908,68 +6915,68 @@
         <v>77</v>
       </c>
       <c r="G169" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H169" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="I169" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="J169" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A170" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B170" s="1" t="s">
+      <c r="A170" t="s">
+        <v>10</v>
+      </c>
+      <c r="B170" t="s">
         <v>41</v>
       </c>
-      <c r="C170" s="1" t="s">
+      <c r="C170" t="s">
         <v>137</v>
       </c>
-      <c r="D170" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F170" s="1" t="s">
+      <c r="D170" t="s">
+        <v>138</v>
+      </c>
+      <c r="E170" t="s">
+        <v>27</v>
+      </c>
+      <c r="F170" t="s">
         <v>77</v>
       </c>
-      <c r="G170" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H170" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I170" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J170" s="1" t="s">
-        <v>26</v>
+      <c r="G170" t="s">
+        <v>14</v>
+      </c>
+      <c r="H170" t="s">
+        <v>14</v>
+      </c>
+      <c r="I170" t="s">
+        <v>14</v>
+      </c>
+      <c r="J170" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B171" t="s">
         <v>41</v>
       </c>
       <c r="C171" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D171" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="E171" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F171" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G171" t="s">
         <v>14</v>
@@ -6985,55 +6992,55 @@
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A172" t="s">
+      <c r="A172" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C172" t="s">
-        <v>141</v>
-      </c>
-      <c r="D172" t="s">
-        <v>142</v>
-      </c>
-      <c r="E172" t="s">
-        <v>15</v>
-      </c>
-      <c r="F172" t="s">
-        <v>16</v>
-      </c>
-      <c r="G172" t="s">
-        <v>14</v>
-      </c>
-      <c r="H172" t="s">
-        <v>14</v>
-      </c>
-      <c r="I172" t="s">
-        <v>14</v>
-      </c>
-      <c r="J172" t="s">
-        <v>14</v>
+      <c r="C172" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I172" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J172" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B173" t="s">
         <v>41</v>
       </c>
       <c r="C173" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D173" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="E173" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F173" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G173" t="s">
         <v>14</v>
@@ -7059,13 +7066,13 @@
         <v>141</v>
       </c>
       <c r="D174" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E174" t="s">
         <v>15</v>
       </c>
       <c r="F174" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="G174" t="s">
         <v>14</v>
@@ -7082,7 +7089,7 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B175" t="s">
         <v>41</v>
@@ -7091,7 +7098,7 @@
         <v>141</v>
       </c>
       <c r="D175" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E175" t="s">
         <v>15</v>
@@ -7114,7 +7121,7 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B176" t="s">
         <v>41</v>
@@ -7123,13 +7130,13 @@
         <v>141</v>
       </c>
       <c r="D176" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E176" t="s">
         <v>15</v>
       </c>
       <c r="F176" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="G176" t="s">
         <v>14</v>
@@ -7146,22 +7153,22 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B177" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="C177" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D177" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
       <c r="E177" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F177" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G177" t="s">
         <v>14</v>
@@ -7178,22 +7185,22 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B178" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="C178" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D178" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E178" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F178" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G178" t="s">
         <v>14</v>
@@ -7219,7 +7226,7 @@
         <v>149</v>
       </c>
       <c r="D179" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="E179" t="s">
         <v>22</v>
@@ -7242,7 +7249,7 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B180" t="s">
         <v>147</v>
@@ -7251,7 +7258,7 @@
         <v>149</v>
       </c>
       <c r="D180" t="s">
-        <v>107</v>
+        <v>150</v>
       </c>
       <c r="E180" t="s">
         <v>22</v>
@@ -7274,7 +7281,7 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B181" t="s">
         <v>147</v>
@@ -7283,7 +7290,7 @@
         <v>149</v>
       </c>
       <c r="D181" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E181" t="s">
         <v>22</v>
@@ -7315,7 +7322,7 @@
         <v>149</v>
       </c>
       <c r="D182" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="E182" t="s">
         <v>22</v>
@@ -7338,22 +7345,22 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B183" t="s">
         <v>147</v>
       </c>
       <c r="C183" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D183" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E183" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F183" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G183" t="s">
         <v>14</v>
@@ -7370,22 +7377,22 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="B184" t="s">
         <v>147</v>
       </c>
       <c r="C184" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D184" t="s">
-        <v>148</v>
+        <v>201</v>
       </c>
       <c r="E184" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F184" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G184" t="s">
         <v>14</v>
@@ -7411,13 +7418,13 @@
         <v>153</v>
       </c>
       <c r="D185" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E185" t="s">
         <v>27</v>
       </c>
       <c r="F185" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="G185" t="s">
         <v>14</v>
@@ -7443,7 +7450,7 @@
         <v>153</v>
       </c>
       <c r="D186" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E186" t="s">
         <v>27</v>
@@ -7466,7 +7473,7 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B187" t="s">
         <v>147</v>
@@ -7475,7 +7482,7 @@
         <v>153</v>
       </c>
       <c r="D187" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E187" t="s">
         <v>27</v>
@@ -7507,7 +7514,7 @@
         <v>153</v>
       </c>
       <c r="D188" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E188" t="s">
         <v>27</v>
@@ -7530,7 +7537,7 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B189" t="s">
         <v>147</v>
@@ -7539,7 +7546,7 @@
         <v>153</v>
       </c>
       <c r="D189" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="E189" t="s">
         <v>27</v>
@@ -7562,7 +7569,7 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B190" t="s">
         <v>147</v>
@@ -7571,7 +7578,7 @@
         <v>153</v>
       </c>
       <c r="D190" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E190" t="s">
         <v>27</v>
@@ -7603,7 +7610,7 @@
         <v>153</v>
       </c>
       <c r="D191" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E191" t="s">
         <v>27</v>
@@ -7635,7 +7642,7 @@
         <v>153</v>
       </c>
       <c r="D192" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E192" t="s">
         <v>27</v>
@@ -7658,16 +7665,16 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B193" t="s">
         <v>147</v>
       </c>
       <c r="C193" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D193" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E193" t="s">
         <v>27</v>
@@ -7690,22 +7697,22 @@
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B194" t="s">
         <v>147</v>
       </c>
       <c r="C194" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D194" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E194" t="s">
         <v>27</v>
       </c>
       <c r="F194" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="G194" t="s">
         <v>14</v>
@@ -7731,13 +7738,13 @@
         <v>157</v>
       </c>
       <c r="D195" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E195" t="s">
         <v>27</v>
       </c>
       <c r="F195" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G195" t="s">
         <v>14</v>
@@ -7763,7 +7770,7 @@
         <v>157</v>
       </c>
       <c r="D196" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E196" t="s">
         <v>27</v>
@@ -7786,7 +7793,7 @@
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B197" t="s">
         <v>147</v>
@@ -7795,13 +7802,13 @@
         <v>157</v>
       </c>
       <c r="D197" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E197" t="s">
         <v>27</v>
       </c>
       <c r="F197" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="G197" t="s">
         <v>14</v>
@@ -7818,7 +7825,7 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B198" t="s">
         <v>147</v>
@@ -7827,13 +7834,13 @@
         <v>157</v>
       </c>
       <c r="D198" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E198" t="s">
         <v>27</v>
       </c>
       <c r="F198" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="G198" t="s">
         <v>14</v>
@@ -7850,7 +7857,7 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B199" t="s">
         <v>147</v>
@@ -7882,7 +7889,7 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B200" t="s">
         <v>147</v>
@@ -7897,7 +7904,7 @@
         <v>27</v>
       </c>
       <c r="F200" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="G200" t="s">
         <v>14</v>
@@ -7914,22 +7921,22 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B201" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="C201" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D201" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E201" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F201" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="G201" t="s">
         <v>14</v>
@@ -7946,22 +7953,22 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B202" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="C202" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D202" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E202" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F202" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G202" t="s">
         <v>14</v>
@@ -7978,7 +7985,7 @@
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B203" t="s">
         <v>162</v>
@@ -7987,7 +7994,7 @@
         <v>163</v>
       </c>
       <c r="D203" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E203" t="s">
         <v>15</v>
@@ -8010,7 +8017,7 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B204" t="s">
         <v>162</v>
@@ -8042,16 +8049,16 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B205" t="s">
         <v>162</v>
       </c>
       <c r="C205" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D205" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="E205" t="s">
         <v>15</v>
@@ -8074,16 +8081,16 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="B206" t="s">
         <v>162</v>
       </c>
       <c r="C206" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D206" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E206" t="s">
         <v>15</v>
@@ -8115,7 +8122,7 @@
         <v>166</v>
       </c>
       <c r="D207" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E207" t="s">
         <v>15</v>
@@ -8138,7 +8145,7 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>173</v>
+        <v>10</v>
       </c>
       <c r="B208" t="s">
         <v>162</v>
@@ -8147,7 +8154,7 @@
         <v>166</v>
       </c>
       <c r="D208" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E208" t="s">
         <v>15</v>
@@ -8176,10 +8183,10 @@
         <v>162</v>
       </c>
       <c r="C209" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D209" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E209" t="s">
         <v>15</v>
@@ -8200,14 +8207,78 @@
         <v>14</v>
       </c>
     </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>173</v>
+      </c>
+      <c r="B210" t="s">
+        <v>162</v>
+      </c>
+      <c r="C210" t="s">
+        <v>166</v>
+      </c>
+      <c r="D210" t="s">
+        <v>153</v>
+      </c>
+      <c r="E210" t="s">
+        <v>15</v>
+      </c>
+      <c r="F210" t="s">
+        <v>16</v>
+      </c>
+      <c r="G210" t="s">
+        <v>14</v>
+      </c>
+      <c r="H210" t="s">
+        <v>14</v>
+      </c>
+      <c r="I210" t="s">
+        <v>14</v>
+      </c>
+      <c r="J210" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>10</v>
+      </c>
+      <c r="B211" t="s">
+        <v>162</v>
+      </c>
+      <c r="C211" t="s">
+        <v>167</v>
+      </c>
+      <c r="D211" t="s">
+        <v>167</v>
+      </c>
+      <c r="E211" t="s">
+        <v>15</v>
+      </c>
+      <c r="F211" t="s">
+        <v>16</v>
+      </c>
+      <c r="G211" t="s">
+        <v>14</v>
+      </c>
+      <c r="H211" t="s">
+        <v>14</v>
+      </c>
+      <c r="I211" t="s">
+        <v>14</v>
+      </c>
+      <c r="J211" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J209" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J209">
-      <sortCondition ref="B1:B209"/>
+  <autoFilter ref="A1:J211" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J211">
+      <sortCondition ref="B1:B211"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:J234">
-    <sortCondition ref="D2:D234"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:J236">
+    <sortCondition ref="D2:D236"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
group update for continuous cover
</commit_message>
<xml_diff>
--- a/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
+++ b/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesley.atwood\Desktop\GitHub\AgEvidence\AgEvidence_Kenya\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E393F7-7E75-4DF7-85FA-92434B9BAAFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE62013D-957C-4A28-90D4-2E1A52D55819}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2334" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2340" uniqueCount="210">
   <si>
     <t>Review</t>
   </si>
@@ -1524,9 +1524,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J234"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C180" sqref="C180:D180"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D238" sqref="D238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6341,7 +6341,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>10</v>
       </c>
@@ -6373,7 +6373,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>10</v>
       </c>
@@ -6405,7 +6405,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>10</v>
       </c>
@@ -6437,7 +6437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="154" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:10" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>10</v>
       </c>
@@ -6469,7 +6469,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>10</v>
       </c>
@@ -6501,7 +6501,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>171</v>
       </c>
@@ -6533,7 +6533,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>10</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>10</v>
       </c>
@@ -6597,7 +6597,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>10</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>10</v>
       </c>
@@ -6661,7 +6661,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>10</v>
       </c>
@@ -6693,7 +6693,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>10</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>10</v>
       </c>
@@ -6757,7 +6757,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>17</v>
       </c>
@@ -6789,7 +6789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>10</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>10</v>
       </c>
@@ -6853,7 +6853,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>10</v>
       </c>
@@ -6885,7 +6885,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>10</v>
       </c>
@@ -6917,7 +6917,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>10</v>
       </c>
@@ -6949,7 +6949,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>10</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>171</v>
       </c>
@@ -7013,7 +7013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -7045,7 +7045,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>171</v>
       </c>
@@ -7077,7 +7077,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>171</v>
       </c>
@@ -7109,7 +7109,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>171</v>
       </c>
@@ -7141,7 +7141,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>171</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="177" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>171</v>
       </c>
@@ -7205,7 +7205,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="178" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" s="3" t="s">
         <v>171</v>
       </c>
@@ -7237,7 +7237,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="179" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" s="3" t="s">
         <v>10</v>
       </c>
@@ -7269,7 +7269,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="180" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" s="3" t="s">
         <v>10</v>
       </c>
@@ -7301,7 +7301,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="181" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" s="3" t="s">
         <v>171</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="182" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" s="3" t="s">
         <v>171</v>
       </c>
@@ -7365,7 +7365,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="183" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="3" t="s">
         <v>10</v>
       </c>
@@ -7397,7 +7397,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="184" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="3" t="s">
         <v>17</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="185" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="3" t="s">
         <v>10</v>
       </c>
@@ -7461,7 +7461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="186" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="3" t="s">
         <v>17</v>
       </c>
@@ -7493,7 +7493,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" s="3" t="s">
         <v>171</v>
       </c>
@@ -7525,7 +7525,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>10</v>
       </c>
@@ -7557,7 +7557,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>10</v>
       </c>
@@ -7589,7 +7589,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>17</v>
       </c>
@@ -7621,7 +7621,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>17</v>
       </c>
@@ -7653,7 +7653,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>17</v>
       </c>
@@ -8485,7 +8485,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>10</v>
       </c>
@@ -8517,7 +8517,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>10</v>
       </c>
@@ -8549,7 +8549,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>17</v>
       </c>
@@ -8581,7 +8581,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>171</v>
       </c>
@@ -8613,7 +8613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>10</v>
       </c>
@@ -8645,7 +8645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>10</v>
       </c>
@@ -8677,7 +8677,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>10</v>
       </c>
@@ -8709,7 +8709,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>171</v>
       </c>
@@ -8741,7 +8741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>10</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>10</v>
       </c>
@@ -8837,7 +8837,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>10</v>
       </c>
@@ -8869,7 +8869,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="230" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>10</v>
       </c>
@@ -8882,8 +8882,26 @@
       <c r="D230" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E230" t="s">
+        <v>15</v>
+      </c>
+      <c r="F230" t="s">
+        <v>77</v>
+      </c>
+      <c r="G230" t="s">
+        <v>14</v>
+      </c>
+      <c r="H230" t="s">
+        <v>14</v>
+      </c>
+      <c r="I230" t="s">
+        <v>14</v>
+      </c>
+      <c r="J230" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>10</v>
       </c>
@@ -8915,7 +8933,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>10</v>
       </c>
@@ -8947,7 +8965,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>10</v>
       </c>
@@ -9015,7 +9033,7 @@
   <autoFilter ref="A1:J234" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Pests"/>
+        <filter val="Water Quality"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J227">

</xml_diff>

<commit_message>
groups updated to match
</commit_message>
<xml_diff>
--- a/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
+++ b/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesley.atwood\Desktop\GitHub\AgEvidence\AgEvidence_Kenya\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E6A887-D9F9-43EF-8945-D6ACDEDA9C1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA4668C-2AD3-4311-A37A-6979E3319629}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39720" yWindow="1845" windowWidth="24885" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1488,8 +1488,8 @@
   <dimension ref="A1:J225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D117" sqref="D117"/>
+      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B184" sqref="B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
normative effect assignments for pest groupings altered so only nematode community data display with soil biotic comm
</commit_message>
<xml_diff>
--- a/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
+++ b/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesley.atwood\Desktop\GitHub\AgEvidence\AgEvidence_Kenya\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA4668C-2AD3-4311-A37A-6979E3319629}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FFFD39-7DC8-4EFD-A74A-F79CC80D2E59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39720" yWindow="1845" windowWidth="24885" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grouplists_Kenya_2021-07-14" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'grouplists_Kenya_2021-07-14'!$A$1:$J$225</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'grouplists_Kenya_2021-07-14'!$A$1:$J$226</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2250" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2260" uniqueCount="198">
   <si>
     <t>Review</t>
   </si>
@@ -1485,11 +1485,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J225"/>
+  <dimension ref="A1:J226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B184" sqref="B184"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1544,10 +1544,10 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -1576,10 +1576,10 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -1602,7 +1602,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -1611,7 +1611,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -1634,7 +1634,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -1643,7 +1643,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1675,7 +1675,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -1698,16 +1698,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -1730,34 +1730,34 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1771,13 +1771,13 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>
@@ -1789,7 +1789,7 @@
         <v>23</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1800,28 +1800,28 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J10" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -1832,28 +1832,28 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>118</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I11" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J11" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1864,10 +1864,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -1899,7 +1899,7 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -1931,7 +1931,7 @@
         <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E14" t="s">
         <v>14</v>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -1963,7 +1963,7 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E15" t="s">
         <v>14</v>
@@ -1986,34 +1986,34 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="I16" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J16" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -2024,60 +2024,60 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="I17" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J17" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="I18" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J18" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -2088,10 +2088,10 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E19" t="s">
         <v>14</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -2152,10 +2152,10 @@
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
@@ -2181,13 +2181,13 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E22" t="s">
         <v>14</v>
@@ -2196,16 +2196,16 @@
         <v>15</v>
       </c>
       <c r="G22" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H22" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="I22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -2216,33 +2216,33 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G23" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H23" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="I23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J23" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
@@ -2274,7 +2274,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -2306,7 +2306,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
@@ -2315,7 +2315,7 @@
         <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -2370,7 +2370,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
@@ -2379,7 +2379,7 @@
         <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="E28" t="s">
         <v>19</v>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
         <v>26</v>
@@ -2411,13 +2411,13 @@
         <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E29" t="s">
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G29" t="s">
         <v>13</v>
@@ -2443,13 +2443,13 @@
         <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="E30" t="s">
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G30" t="s">
         <v>13</v>
@@ -2466,7 +2466,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
         <v>26</v>
@@ -2498,7 +2498,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B32" t="s">
         <v>26</v>
@@ -2530,7 +2530,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
         <v>26</v>
@@ -2539,7 +2539,7 @@
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
@@ -2562,7 +2562,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B34" t="s">
         <v>26</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
         <v>26</v>
@@ -2603,7 +2603,7 @@
         <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E35" t="s">
         <v>19</v>
@@ -2626,16 +2626,16 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
         <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E36" t="s">
         <v>19</v>
@@ -2658,16 +2658,16 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
         <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E37" t="s">
         <v>19</v>
@@ -2699,7 +2699,7 @@
         <v>32</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
@@ -2731,7 +2731,7 @@
         <v>32</v>
       </c>
       <c r="D39" t="s">
-        <v>132</v>
+        <v>33</v>
       </c>
       <c r="E39" t="s">
         <v>19</v>
@@ -2760,10 +2760,10 @@
         <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D40" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
       <c r="E40" t="s">
         <v>19</v>
@@ -2792,10 +2792,10 @@
         <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D41" t="s">
-        <v>110</v>
+        <v>39</v>
       </c>
       <c r="E41" t="s">
         <v>19</v>
@@ -2818,22 +2818,22 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
         <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D42" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="E42" t="s">
         <v>19</v>
       </c>
       <c r="F42" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G42" t="s">
         <v>13</v>
@@ -2859,13 +2859,13 @@
         <v>51</v>
       </c>
       <c r="D43" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="E43" t="s">
         <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G43" t="s">
         <v>13</v>
@@ -2891,13 +2891,13 @@
         <v>51</v>
       </c>
       <c r="D44" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G44" t="s">
         <v>13</v>
@@ -2914,7 +2914,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
         <v>26</v>
@@ -2955,7 +2955,7 @@
         <v>51</v>
       </c>
       <c r="D46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
@@ -2987,13 +2987,13 @@
         <v>51</v>
       </c>
       <c r="D47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
       </c>
       <c r="F47" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G47" t="s">
         <v>13</v>
@@ -3019,7 +3019,7 @@
         <v>51</v>
       </c>
       <c r="D48" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
@@ -3042,7 +3042,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
         <v>26</v>
@@ -3051,7 +3051,7 @@
         <v>51</v>
       </c>
       <c r="D49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E49" t="s">
         <v>19</v>
@@ -3074,7 +3074,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
         <v>26</v>
@@ -3106,7 +3106,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B51" t="s">
         <v>26</v>
@@ -3115,13 +3115,13 @@
         <v>51</v>
       </c>
       <c r="D51" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="E51" t="s">
         <v>19</v>
       </c>
       <c r="F51" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G51" t="s">
         <v>13</v>
@@ -3138,7 +3138,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
         <v>26</v>
@@ -3153,7 +3153,7 @@
         <v>19</v>
       </c>
       <c r="F52" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G52" t="s">
         <v>13</v>
@@ -3170,7 +3170,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B53" t="s">
         <v>26</v>
@@ -3179,7 +3179,7 @@
         <v>51</v>
       </c>
       <c r="D53" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E53" t="s">
         <v>19</v>
@@ -3211,7 +3211,7 @@
         <v>51</v>
       </c>
       <c r="D54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E54" t="s">
         <v>19</v>
@@ -3240,10 +3240,10 @@
         <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D55" t="s">
-        <v>54</v>
+        <v>139</v>
       </c>
       <c r="E55" t="s">
         <v>19</v>
@@ -3266,22 +3266,22 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B56" t="s">
         <v>26</v>
       </c>
       <c r="C56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D56" t="s">
         <v>54</v>
       </c>
       <c r="E56" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G56" t="s">
         <v>13</v>
@@ -3307,7 +3307,7 @@
         <v>53</v>
       </c>
       <c r="D57" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E57" t="s">
         <v>14</v>
@@ -3330,22 +3330,22 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B58" t="s">
         <v>26</v>
       </c>
       <c r="C58" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D58" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="E58" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F58" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G58" t="s">
         <v>13</v>
@@ -3362,16 +3362,16 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B59" t="s">
         <v>26</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" t="s">
         <v>55</v>
       </c>
       <c r="D59" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="E59" t="s">
         <v>19</v>
@@ -3394,12 +3394,12 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B60" t="s">
         <v>26</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D60" t="s">
@@ -3426,7 +3426,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B61" t="s">
         <v>26</v>
@@ -3458,16 +3458,16 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B62" t="s">
         <v>26</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" t="s">
         <v>55</v>
       </c>
       <c r="D62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E62" t="s">
         <v>19</v>
@@ -3499,7 +3499,7 @@
         <v>55</v>
       </c>
       <c r="D63" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
@@ -3531,7 +3531,7 @@
         <v>55</v>
       </c>
       <c r="D64" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E64" t="s">
         <v>19</v>
@@ -3563,7 +3563,7 @@
         <v>55</v>
       </c>
       <c r="D65" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
@@ -3595,7 +3595,7 @@
         <v>55</v>
       </c>
       <c r="D66" t="s">
-        <v>140</v>
+        <v>39</v>
       </c>
       <c r="E66" t="s">
         <v>19</v>
@@ -3627,7 +3627,7 @@
         <v>55</v>
       </c>
       <c r="D67" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E67" t="s">
         <v>19</v>
@@ -3659,7 +3659,7 @@
         <v>55</v>
       </c>
       <c r="D68" t="s">
-        <v>40</v>
+        <v>141</v>
       </c>
       <c r="E68" t="s">
         <v>19</v>
@@ -3687,11 +3687,11 @@
       <c r="B69" t="s">
         <v>26</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D69" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E69" t="s">
         <v>19</v>
@@ -3714,7 +3714,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B70" t="s">
         <v>26</v>
@@ -3746,7 +3746,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B71" t="s">
         <v>26</v>
@@ -3778,16 +3778,16 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B72" t="s">
         <v>26</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" t="s">
         <v>55</v>
       </c>
       <c r="D72" t="s">
-        <v>142</v>
+        <v>41</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
@@ -3819,7 +3819,7 @@
         <v>55</v>
       </c>
       <c r="D73" t="s">
-        <v>42</v>
+        <v>142</v>
       </c>
       <c r="E73" t="s">
         <v>19</v>
@@ -3851,7 +3851,7 @@
         <v>55</v>
       </c>
       <c r="D74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E74" t="s">
         <v>19</v>
@@ -3883,7 +3883,7 @@
         <v>55</v>
       </c>
       <c r="D75" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E75" t="s">
         <v>19</v>
@@ -3911,11 +3911,11 @@
       <c r="B76" t="s">
         <v>26</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D76" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E76" t="s">
         <v>19</v>
@@ -3947,7 +3947,7 @@
         <v>55</v>
       </c>
       <c r="D77" t="s">
-        <v>143</v>
+        <v>45</v>
       </c>
       <c r="E77" t="s">
         <v>19</v>
@@ -3975,11 +3975,11 @@
       <c r="B78" t="s">
         <v>26</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" t="s">
         <v>55</v>
       </c>
       <c r="D78" t="s">
-        <v>46</v>
+        <v>143</v>
       </c>
       <c r="E78" t="s">
         <v>19</v>
@@ -4011,7 +4011,7 @@
         <v>55</v>
       </c>
       <c r="D79" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
       <c r="E79" t="s">
         <v>19</v>
@@ -4039,11 +4039,11 @@
       <c r="B80" t="s">
         <v>26</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D80" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
@@ -4066,7 +4066,7 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B81" t="s">
         <v>26</v>
@@ -4098,7 +4098,7 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B82" t="s">
         <v>26</v>
@@ -4130,16 +4130,16 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B83" t="s">
         <v>26</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" t="s">
         <v>55</v>
       </c>
       <c r="D83" t="s">
-        <v>145</v>
+        <v>34</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
@@ -4171,7 +4171,7 @@
         <v>55</v>
       </c>
       <c r="D84" t="s">
-        <v>47</v>
+        <v>145</v>
       </c>
       <c r="E84" t="s">
         <v>19</v>
@@ -4194,34 +4194,34 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>56</v>
-      </c>
-      <c r="C85" t="s">
-        <v>95</v>
+        <v>26</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D85" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="E85" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F85" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G85" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H85" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="I85" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J85" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
@@ -4232,28 +4232,28 @@
         <v>56</v>
       </c>
       <c r="C86" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="D86" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="E86" t="s">
         <v>14</v>
       </c>
       <c r="F86" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G86" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H86" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="I86" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J86" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
@@ -4267,13 +4267,13 @@
         <v>57</v>
       </c>
       <c r="D87" t="s">
-        <v>96</v>
+        <v>146</v>
       </c>
       <c r="E87" t="s">
         <v>14</v>
       </c>
       <c r="F87" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G87" t="s">
         <v>13</v>
@@ -4299,13 +4299,13 @@
         <v>57</v>
       </c>
       <c r="D88" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
       <c r="E88" t="s">
         <v>14</v>
       </c>
       <c r="F88" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G88" t="s">
         <v>13</v>
@@ -4322,7 +4322,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B89" t="s">
         <v>56</v>
@@ -4331,13 +4331,13 @@
         <v>57</v>
       </c>
       <c r="D89" t="s">
-        <v>58</v>
+        <v>147</v>
       </c>
       <c r="E89" t="s">
         <v>14</v>
       </c>
       <c r="F89" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G89" t="s">
         <v>13</v>
@@ -4354,7 +4354,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B90" t="s">
         <v>56</v>
@@ -4386,7 +4386,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B91" t="s">
         <v>56</v>
@@ -4395,7 +4395,7 @@
         <v>57</v>
       </c>
       <c r="D91" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
       <c r="E91" t="s">
         <v>14</v>
@@ -4416,9 +4416,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B92" t="s">
         <v>56</v>
@@ -4448,82 +4448,82 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="3" t="s">
+    <row r="93" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
         <v>93</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" t="s">
         <v>56</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" t="s">
         <v>57</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D93" t="s">
+        <v>148</v>
+      </c>
+      <c r="E93" t="s">
+        <v>14</v>
+      </c>
+      <c r="F93" t="s">
+        <v>15</v>
+      </c>
+      <c r="G93" t="s">
+        <v>13</v>
+      </c>
+      <c r="H93" t="s">
+        <v>13</v>
+      </c>
+      <c r="I93" t="s">
+        <v>13</v>
+      </c>
+      <c r="J93" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D94" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E93" s="3" t="s">
+      <c r="E94" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F93" s="3" t="s">
+      <c r="F94" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G93" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H93" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I93" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J93" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+      <c r="G94" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J94" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
         <v>16</v>
       </c>
-      <c r="B94" t="s">
-        <v>56</v>
-      </c>
-      <c r="C94" t="s">
-        <v>59</v>
-      </c>
-      <c r="D94" t="s">
-        <v>150</v>
-      </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
-      <c r="F94" t="s">
-        <v>22</v>
-      </c>
-      <c r="G94" t="s">
-        <v>13</v>
-      </c>
-      <c r="H94" t="s">
-        <v>13</v>
-      </c>
-      <c r="I94" t="s">
-        <v>13</v>
-      </c>
-      <c r="J94" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A95" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" t="s">
         <v>56</v>
       </c>
       <c r="C95" t="s">
         <v>59</v>
       </c>
       <c r="D95" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E95" t="s">
         <v>19</v>
@@ -4531,24 +4531,24 @@
       <c r="F95" t="s">
         <v>22</v>
       </c>
-      <c r="G95" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J95" s="1" t="s">
+      <c r="G95" t="s">
+        <v>13</v>
+      </c>
+      <c r="H95" t="s">
+        <v>13</v>
+      </c>
+      <c r="I95" t="s">
+        <v>13</v>
+      </c>
+      <c r="J95" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
-        <v>16</v>
-      </c>
-      <c r="B96" t="s">
+      <c r="A96" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C96" t="s">
@@ -4563,22 +4563,22 @@
       <c r="F96" t="s">
         <v>22</v>
       </c>
-      <c r="G96" t="s">
-        <v>13</v>
-      </c>
-      <c r="H96" t="s">
-        <v>13</v>
-      </c>
-      <c r="I96" t="s">
-        <v>13</v>
-      </c>
-      <c r="J96" t="s">
+      <c r="G96" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J96" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B97" t="s">
         <v>56</v>
@@ -4587,7 +4587,7 @@
         <v>59</v>
       </c>
       <c r="D97" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E97" t="s">
         <v>19</v>
@@ -4616,16 +4616,16 @@
         <v>56</v>
       </c>
       <c r="C98" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D98" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E98" t="s">
         <v>19</v>
       </c>
       <c r="F98" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G98" t="s">
         <v>13</v>
@@ -4642,19 +4642,19 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B99" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C99" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D99" t="s">
-        <v>61</v>
+        <v>153</v>
       </c>
       <c r="E99" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F99" t="s">
         <v>50</v>
@@ -4674,7 +4674,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B100" t="s">
         <v>20</v>
@@ -4683,7 +4683,7 @@
         <v>60</v>
       </c>
       <c r="D100" t="s">
-        <v>154</v>
+        <v>61</v>
       </c>
       <c r="E100" t="s">
         <v>23</v>
@@ -4715,7 +4715,7 @@
         <v>60</v>
       </c>
       <c r="D101" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E101" t="s">
         <v>23</v>
@@ -4738,7 +4738,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B102" t="s">
         <v>20</v>
@@ -4770,7 +4770,7 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B103" t="s">
         <v>20</v>
@@ -4802,7 +4802,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B104" t="s">
         <v>20</v>
@@ -4811,7 +4811,7 @@
         <v>60</v>
       </c>
       <c r="D104" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
       <c r="E104" t="s">
         <v>23</v>
@@ -4834,7 +4834,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B105" t="s">
         <v>20</v>
@@ -4866,16 +4866,16 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B106" t="s">
         <v>20</v>
       </c>
       <c r="C106" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D106" t="s">
-        <v>156</v>
+        <v>102</v>
       </c>
       <c r="E106" t="s">
         <v>23</v>
@@ -4898,7 +4898,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B107" t="s">
         <v>20</v>
@@ -4930,7 +4930,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B108" t="s">
         <v>20</v>
@@ -4939,7 +4939,7 @@
         <v>62</v>
       </c>
       <c r="D108" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E108" t="s">
         <v>23</v>
@@ -4971,13 +4971,13 @@
         <v>62</v>
       </c>
       <c r="D109" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E109" t="s">
         <v>23</v>
       </c>
       <c r="F109" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G109" t="s">
         <v>13</v>
@@ -4994,7 +4994,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B110" t="s">
         <v>20</v>
@@ -5026,7 +5026,7 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B111" t="s">
         <v>20</v>
@@ -5058,7 +5058,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B112" t="s">
         <v>20</v>
@@ -5067,7 +5067,7 @@
         <v>62</v>
       </c>
       <c r="D112" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E112" t="s">
         <v>23</v>
@@ -5090,7 +5090,7 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B113" t="s">
         <v>20</v>
@@ -5131,13 +5131,13 @@
         <v>62</v>
       </c>
       <c r="D114" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E114" t="s">
         <v>23</v>
       </c>
       <c r="F114" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G114" t="s">
         <v>13</v>
@@ -5154,7 +5154,7 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B115" t="s">
         <v>20</v>
@@ -5163,13 +5163,13 @@
         <v>62</v>
       </c>
       <c r="D115" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E115" t="s">
         <v>23</v>
       </c>
       <c r="F115" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G115" t="s">
         <v>13</v>
@@ -5186,7 +5186,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B116" t="s">
         <v>20</v>
@@ -5218,7 +5218,7 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B117" t="s">
         <v>20</v>
@@ -5227,7 +5227,7 @@
         <v>62</v>
       </c>
       <c r="D117" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="E117" t="s">
         <v>23</v>
@@ -5250,7 +5250,7 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B118" t="s">
         <v>20</v>
@@ -5282,7 +5282,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B119" t="s">
         <v>20</v>
@@ -5291,7 +5291,7 @@
         <v>62</v>
       </c>
       <c r="D119" t="s">
-        <v>94</v>
+        <v>197</v>
       </c>
       <c r="E119" t="s">
         <v>23</v>
@@ -5300,21 +5300,21 @@
         <v>50</v>
       </c>
       <c r="G119" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H119" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I119" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J119" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B120" t="s">
         <v>20</v>
@@ -5346,34 +5346,34 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B121" t="s">
         <v>20</v>
       </c>
       <c r="C121" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="D121" t="s">
-        <v>162</v>
+        <v>94</v>
       </c>
       <c r="E121" t="s">
         <v>23</v>
       </c>
       <c r="F121" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G121" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H121" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J121" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.35">
@@ -5387,7 +5387,7 @@
         <v>21</v>
       </c>
       <c r="D122" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E122" t="s">
         <v>23</v>
@@ -5396,16 +5396,16 @@
         <v>22</v>
       </c>
       <c r="G122" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H122" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I122" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J122" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.35">
@@ -5419,7 +5419,7 @@
         <v>21</v>
       </c>
       <c r="D123" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E123" t="s">
         <v>23</v>
@@ -5428,21 +5428,21 @@
         <v>22</v>
       </c>
       <c r="G123" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H123" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I123" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J123" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B124" t="s">
         <v>20</v>
@@ -5451,13 +5451,13 @@
         <v>21</v>
       </c>
       <c r="D124" t="s">
-        <v>64</v>
+        <v>164</v>
       </c>
       <c r="E124" t="s">
         <v>23</v>
       </c>
       <c r="F124" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G124" t="s">
         <v>13</v>
@@ -5474,7 +5474,7 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B125" t="s">
         <v>20</v>
@@ -5506,7 +5506,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B126" t="s">
         <v>20</v>
@@ -5538,7 +5538,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B127" t="s">
         <v>20</v>
@@ -5547,30 +5547,30 @@
         <v>21</v>
       </c>
       <c r="D127" t="s">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="E127" t="s">
         <v>23</v>
       </c>
       <c r="F127" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G127" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H127" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I127" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J127" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B128" t="s">
         <v>20</v>
@@ -5579,7 +5579,7 @@
         <v>21</v>
       </c>
       <c r="D128" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="E128" t="s">
         <v>23</v>
@@ -5602,7 +5602,7 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B129" t="s">
         <v>20</v>
@@ -5634,7 +5634,7 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B130" t="s">
         <v>20</v>
@@ -5666,39 +5666,39 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B131" t="s">
         <v>20</v>
       </c>
       <c r="C131" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="D131" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E131" t="s">
         <v>23</v>
       </c>
       <c r="F131" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G131" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H131" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I131" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J131" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B132" t="s">
         <v>20</v>
@@ -5707,13 +5707,13 @@
         <v>65</v>
       </c>
       <c r="D132" t="s">
-        <v>67</v>
+        <v>166</v>
       </c>
       <c r="E132" t="s">
         <v>23</v>
       </c>
       <c r="F132" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G132" t="s">
         <v>13</v>
@@ -5730,7 +5730,7 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B133" t="s">
         <v>20</v>
@@ -5739,7 +5739,7 @@
         <v>65</v>
       </c>
       <c r="D133" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E133" t="s">
         <v>23</v>
@@ -5748,21 +5748,21 @@
         <v>15</v>
       </c>
       <c r="G133" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H133" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="I133" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J133" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B134" t="s">
         <v>20</v>
@@ -5780,21 +5780,21 @@
         <v>15</v>
       </c>
       <c r="G134" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H134" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="I134" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J134" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B135" t="s">
         <v>20</v>
@@ -5835,13 +5835,13 @@
         <v>65</v>
       </c>
       <c r="D136" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E136" t="s">
         <v>23</v>
       </c>
       <c r="F136" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G136" t="s">
         <v>13</v>
@@ -5858,7 +5858,7 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B137" t="s">
         <v>20</v>
@@ -5896,13 +5896,13 @@
         <v>20</v>
       </c>
       <c r="C138" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D138" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E138" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F138" t="s">
         <v>22</v>
@@ -5922,7 +5922,7 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B139" t="s">
         <v>20</v>
@@ -5954,7 +5954,7 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B140" t="s">
         <v>20</v>
@@ -5986,7 +5986,7 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B141" t="s">
         <v>20</v>
@@ -5995,7 +5995,7 @@
         <v>66</v>
       </c>
       <c r="D141" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E141" t="s">
         <v>19</v>
@@ -6018,7 +6018,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B142" t="s">
         <v>20</v>
@@ -6050,22 +6050,22 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B143" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C143" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="D143" t="s">
-        <v>107</v>
+        <v>170</v>
       </c>
       <c r="E143" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F143" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G143" t="s">
         <v>13</v>
@@ -6088,10 +6088,10 @@
         <v>28</v>
       </c>
       <c r="C144" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="D144" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="E144" t="s">
         <v>14</v>
@@ -6100,16 +6100,16 @@
         <v>15</v>
       </c>
       <c r="G144" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="H144" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="I144" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J144" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.35">
@@ -6123,7 +6123,7 @@
         <v>27</v>
       </c>
       <c r="D145" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E145" t="s">
         <v>14</v>
@@ -6144,7 +6144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>10</v>
       </c>
@@ -6155,7 +6155,7 @@
         <v>27</v>
       </c>
       <c r="D146" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E146" t="s">
         <v>14</v>
@@ -6176,7 +6176,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>10</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>27</v>
       </c>
       <c r="D147" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E147" t="s">
         <v>14</v>
@@ -6219,7 +6219,7 @@
         <v>27</v>
       </c>
       <c r="D148" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E148" t="s">
         <v>14</v>
@@ -6242,7 +6242,7 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B149" t="s">
         <v>28</v>
@@ -6251,7 +6251,7 @@
         <v>27</v>
       </c>
       <c r="D149" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E149" t="s">
         <v>14</v>
@@ -6274,16 +6274,16 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B150" t="s">
         <v>28</v>
       </c>
       <c r="C150" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D150" t="s">
-        <v>68</v>
+        <v>176</v>
       </c>
       <c r="E150" t="s">
         <v>14</v>
@@ -6292,16 +6292,16 @@
         <v>15</v>
       </c>
       <c r="G150" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="H150" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="I150" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J150" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.35">
@@ -6315,7 +6315,7 @@
         <v>29</v>
       </c>
       <c r="D151" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="E151" t="s">
         <v>14</v>
@@ -6347,7 +6347,7 @@
         <v>29</v>
       </c>
       <c r="D152" t="s">
-        <v>177</v>
+        <v>105</v>
       </c>
       <c r="E152" t="s">
         <v>14</v>
@@ -6379,7 +6379,7 @@
         <v>29</v>
       </c>
       <c r="D153" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E153" t="s">
         <v>14</v>
@@ -6411,7 +6411,7 @@
         <v>29</v>
       </c>
       <c r="D154" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E154" t="s">
         <v>14</v>
@@ -6434,7 +6434,7 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B155" t="s">
         <v>28</v>
@@ -6443,7 +6443,7 @@
         <v>29</v>
       </c>
       <c r="D155" t="s">
-        <v>69</v>
+        <v>179</v>
       </c>
       <c r="E155" t="s">
         <v>14</v>
@@ -6466,7 +6466,7 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B156" t="s">
         <v>28</v>
@@ -6475,7 +6475,7 @@
         <v>29</v>
       </c>
       <c r="D156" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E156" t="s">
         <v>14</v>
@@ -6498,34 +6498,34 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B157" t="s">
         <v>28</v>
       </c>
       <c r="C157" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="D157" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="E157" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F157" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G157" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H157" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="I157" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J157" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.35">
@@ -6539,7 +6539,7 @@
         <v>71</v>
       </c>
       <c r="D158" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E158" t="s">
         <v>23</v>
@@ -6548,21 +6548,21 @@
         <v>22</v>
       </c>
       <c r="G158" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H158" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="I158" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J158" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B159" t="s">
         <v>28</v>
@@ -6571,13 +6571,13 @@
         <v>71</v>
       </c>
       <c r="D159" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="E159" t="s">
         <v>23</v>
       </c>
       <c r="F159" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G159" t="s">
         <v>13</v>
@@ -6594,7 +6594,7 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B160" t="s">
         <v>28</v>
@@ -6626,7 +6626,7 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B161" t="s">
         <v>28</v>
@@ -6635,25 +6635,25 @@
         <v>71</v>
       </c>
       <c r="D161" t="s">
-        <v>180</v>
+        <v>72</v>
       </c>
       <c r="E161" t="s">
         <v>23</v>
       </c>
       <c r="F161" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G161" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H161" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="I161" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J161" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.35">
@@ -6667,13 +6667,13 @@
         <v>71</v>
       </c>
       <c r="D162" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E162" t="s">
         <v>23</v>
       </c>
       <c r="F162" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G162" t="s">
         <v>20</v>
@@ -6685,12 +6685,12 @@
         <v>23</v>
       </c>
       <c r="J162" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B163" t="s">
         <v>28</v>
@@ -6722,7 +6722,7 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B164" t="s">
         <v>28</v>
@@ -6731,7 +6731,7 @@
         <v>71</v>
       </c>
       <c r="D164" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E164" t="s">
         <v>23</v>
@@ -6754,7 +6754,7 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B165" t="s">
         <v>28</v>
@@ -6769,7 +6769,7 @@
         <v>23</v>
       </c>
       <c r="F165" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G165" t="s">
         <v>20</v>
@@ -6781,12 +6781,12 @@
         <v>23</v>
       </c>
       <c r="J165" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B166" t="s">
         <v>28</v>
@@ -6795,13 +6795,13 @@
         <v>71</v>
       </c>
       <c r="D166" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E166" t="s">
         <v>23</v>
       </c>
       <c r="F166" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G166" t="s">
         <v>20</v>
@@ -6813,12 +6813,12 @@
         <v>23</v>
       </c>
       <c r="J166" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B167" t="s">
         <v>28</v>
@@ -6859,7 +6859,7 @@
         <v>71</v>
       </c>
       <c r="D168" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
       <c r="E168" t="s">
         <v>23</v>
@@ -6880,9 +6880,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="169" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B169" t="s">
         <v>28</v>
@@ -6891,88 +6891,88 @@
         <v>71</v>
       </c>
       <c r="D169" t="s">
+        <v>99</v>
+      </c>
+      <c r="E169" t="s">
+        <v>23</v>
+      </c>
+      <c r="F169" t="s">
+        <v>22</v>
+      </c>
+      <c r="G169" t="s">
+        <v>13</v>
+      </c>
+      <c r="H169" t="s">
+        <v>13</v>
+      </c>
+      <c r="I169" t="s">
+        <v>13</v>
+      </c>
+      <c r="J169" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>10</v>
+      </c>
+      <c r="B170" t="s">
+        <v>28</v>
+      </c>
+      <c r="C170" t="s">
+        <v>71</v>
+      </c>
+      <c r="D170" t="s">
         <v>184</v>
       </c>
-      <c r="E169" t="s">
-        <v>23</v>
-      </c>
-      <c r="F169" t="s">
+      <c r="E170" t="s">
+        <v>23</v>
+      </c>
+      <c r="F170" t="s">
         <v>15</v>
       </c>
-      <c r="G169" t="s">
-        <v>13</v>
-      </c>
-      <c r="H169" t="s">
-        <v>13</v>
-      </c>
-      <c r="I169" t="s">
-        <v>13</v>
-      </c>
-      <c r="J169" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="170" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A170" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B170" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D170" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E170" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F170" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G170" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H170" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I170" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J170" s="3" t="s">
-        <v>50</v>
+      <c r="G170" t="s">
+        <v>13</v>
+      </c>
+      <c r="H170" t="s">
+        <v>13</v>
+      </c>
+      <c r="I170" t="s">
+        <v>13</v>
+      </c>
+      <c r="J170" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="171" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A171" s="3" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F171" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G171" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H171" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I171" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J171" s="3" t="s">
+      <c r="F171" t="s">
+        <v>22</v>
+      </c>
+      <c r="G171" t="s">
+        <v>13</v>
+      </c>
+      <c r="H171" t="s">
+        <v>13</v>
+      </c>
+      <c r="I171" t="s">
+        <v>13</v>
+      </c>
+      <c r="J171" t="s">
         <v>13</v>
       </c>
     </row>
@@ -6987,13 +6987,13 @@
         <v>73</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>185</v>
+        <v>103</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F172" s="3" t="s">
-        <v>50</v>
+      <c r="F172" t="s">
+        <v>22</v>
       </c>
       <c r="G172" s="3" t="s">
         <v>13</v>
@@ -7010,7 +7010,7 @@
     </row>
     <row r="173" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A173" s="3" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>28</v>
@@ -7019,13 +7019,13 @@
         <v>73</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>74</v>
+        <v>185</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F173" s="3" t="s">
-        <v>50</v>
+      <c r="F173" t="s">
+        <v>22</v>
       </c>
       <c r="G173" s="3" t="s">
         <v>13</v>
@@ -7042,7 +7042,7 @@
     </row>
     <row r="174" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A174" s="3" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>28</v>
@@ -7074,7 +7074,7 @@
     </row>
     <row r="175" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A175" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>28</v>
@@ -7106,7 +7106,7 @@
     </row>
     <row r="176" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A176" s="3" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>28</v>
@@ -7115,7 +7115,7 @@
         <v>73</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>23</v>
@@ -7124,21 +7124,21 @@
         <v>50</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H176" s="3" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="I176" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J176" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="177" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A177" s="3" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>28</v>
@@ -7152,8 +7152,8 @@
       <c r="E177" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F177" s="3" t="s">
-        <v>50</v>
+      <c r="F177" t="s">
+        <v>22</v>
       </c>
       <c r="G177" s="3" t="s">
         <v>20</v>
@@ -7170,7 +7170,7 @@
     </row>
     <row r="178" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A178" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>28</v>
@@ -7184,8 +7184,8 @@
       <c r="E178" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F178" s="3" t="s">
-        <v>50</v>
+      <c r="F178" t="s">
+        <v>22</v>
       </c>
       <c r="G178" s="3" t="s">
         <v>20</v>
@@ -7200,67 +7200,67 @@
         <v>22</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A179" s="3" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>186</v>
+        <v>75</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F179" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F179" t="s">
         <v>22</v>
       </c>
       <c r="G179" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H179" s="3" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="I179" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J179" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A180" t="s">
-        <v>10</v>
-      </c>
-      <c r="B180" t="s">
+      <c r="A180" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B180" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C180" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D180" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E180" t="s">
-        <v>19</v>
-      </c>
-      <c r="F180" t="s">
-        <v>22</v>
-      </c>
-      <c r="G180" t="s">
-        <v>13</v>
-      </c>
-      <c r="H180" t="s">
-        <v>13</v>
-      </c>
-      <c r="I180" t="s">
-        <v>13</v>
-      </c>
-      <c r="J180" t="s">
+      <c r="E180" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G180" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H180" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I180" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J180" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -7274,8 +7274,8 @@
       <c r="C181" t="s">
         <v>76</v>
       </c>
-      <c r="D181" t="s">
-        <v>187</v>
+      <c r="D181" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="E181" t="s">
         <v>19</v>
@@ -7298,22 +7298,22 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B182" t="s">
         <v>28</v>
       </c>
       <c r="C182" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D182" t="s">
-        <v>78</v>
+        <v>187</v>
       </c>
       <c r="E182" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F182" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G182" t="s">
         <v>13</v>
@@ -7330,7 +7330,7 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B183" t="s">
         <v>28</v>
@@ -7362,7 +7362,7 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B184" t="s">
         <v>28</v>
@@ -7371,7 +7371,7 @@
         <v>77</v>
       </c>
       <c r="D184" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E184" t="s">
         <v>14</v>
@@ -7394,7 +7394,7 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B185" t="s">
         <v>28</v>
@@ -7435,7 +7435,7 @@
         <v>77</v>
       </c>
       <c r="D186" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="E186" t="s">
         <v>14</v>
@@ -7467,7 +7467,7 @@
         <v>77</v>
       </c>
       <c r="D187" t="s">
-        <v>188</v>
+        <v>112</v>
       </c>
       <c r="E187" t="s">
         <v>14</v>
@@ -7490,7 +7490,7 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B188" t="s">
         <v>28</v>
@@ -7499,13 +7499,13 @@
         <v>77</v>
       </c>
       <c r="D188" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E188" t="s">
         <v>14</v>
       </c>
       <c r="F188" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G188" t="s">
         <v>13</v>
@@ -7522,7 +7522,7 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B189" t="s">
         <v>28</v>
@@ -7554,22 +7554,22 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B190" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="C190" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="D190" t="s">
-        <v>63</v>
+        <v>189</v>
       </c>
       <c r="E190" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F190" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G190" t="s">
         <v>13</v>
@@ -7586,7 +7586,7 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B191" t="s">
         <v>80</v>
@@ -7618,7 +7618,7 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B192" t="s">
         <v>80</v>
@@ -7627,7 +7627,7 @@
         <v>113</v>
       </c>
       <c r="D192" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="E192" t="s">
         <v>19</v>
@@ -7650,7 +7650,7 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B193" t="s">
         <v>80</v>
@@ -7682,7 +7682,7 @@
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B194" t="s">
         <v>80</v>
@@ -7691,7 +7691,7 @@
         <v>113</v>
       </c>
       <c r="D194" t="s">
-        <v>190</v>
+        <v>82</v>
       </c>
       <c r="E194" t="s">
         <v>19</v>
@@ -7714,7 +7714,7 @@
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B195" t="s">
         <v>80</v>
@@ -7746,7 +7746,7 @@
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B196" t="s">
         <v>80</v>
@@ -7778,22 +7778,22 @@
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B197" t="s">
         <v>80</v>
       </c>
       <c r="C197" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="D197" t="s">
-        <v>81</v>
+        <v>190</v>
       </c>
       <c r="E197" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F197" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G197" t="s">
         <v>13</v>
@@ -7810,7 +7810,7 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B198" t="s">
         <v>80</v>
@@ -7842,7 +7842,7 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B199" t="s">
         <v>80</v>
@@ -7851,7 +7851,7 @@
         <v>84</v>
       </c>
       <c r="D199" t="s">
-        <v>133</v>
+        <v>81</v>
       </c>
       <c r="E199" t="s">
         <v>23</v>
@@ -7874,7 +7874,7 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B200" t="s">
         <v>80</v>
@@ -7906,7 +7906,7 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B201" t="s">
         <v>80</v>
@@ -7938,7 +7938,7 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B202" t="s">
         <v>80</v>
@@ -7947,7 +7947,7 @@
         <v>84</v>
       </c>
       <c r="D202" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="E202" t="s">
         <v>23</v>
@@ -7970,7 +7970,7 @@
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B203" t="s">
         <v>80</v>
@@ -8002,7 +8002,7 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B204" t="s">
         <v>80</v>
@@ -8011,13 +8011,13 @@
         <v>84</v>
       </c>
       <c r="D204" t="s">
-        <v>191</v>
+        <v>83</v>
       </c>
       <c r="E204" t="s">
         <v>23</v>
       </c>
       <c r="F204" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G204" t="s">
         <v>13</v>
@@ -8043,13 +8043,13 @@
         <v>84</v>
       </c>
       <c r="D205" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E205" t="s">
         <v>23</v>
       </c>
       <c r="F205" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G205" t="s">
         <v>13</v>
@@ -8066,7 +8066,7 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B206" t="s">
         <v>80</v>
@@ -8098,7 +8098,7 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B207" t="s">
         <v>80</v>
@@ -8130,16 +8130,16 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B208" t="s">
         <v>80</v>
       </c>
       <c r="C208" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D208" t="s">
-        <v>86</v>
+        <v>192</v>
       </c>
       <c r="E208" t="s">
         <v>23</v>
@@ -8162,7 +8162,7 @@
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B209" t="s">
         <v>80</v>
@@ -8194,7 +8194,7 @@
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B210" t="s">
         <v>80</v>
@@ -8226,7 +8226,7 @@
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B211" t="s">
         <v>80</v>
@@ -8235,13 +8235,13 @@
         <v>85</v>
       </c>
       <c r="D211" t="s">
-        <v>193</v>
+        <v>86</v>
       </c>
       <c r="E211" t="s">
         <v>23</v>
       </c>
       <c r="F211" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G211" t="s">
         <v>13</v>
@@ -8267,13 +8267,13 @@
         <v>85</v>
       </c>
       <c r="D212" t="s">
-        <v>87</v>
+        <v>193</v>
       </c>
       <c r="E212" t="s">
         <v>23</v>
       </c>
       <c r="F212" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G212" t="s">
         <v>13</v>
@@ -8290,7 +8290,7 @@
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B213" t="s">
         <v>80</v>
@@ -8305,7 +8305,7 @@
         <v>23</v>
       </c>
       <c r="F213" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G213" t="s">
         <v>13</v>
@@ -8322,7 +8322,7 @@
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B214" t="s">
         <v>80</v>
@@ -8337,7 +8337,7 @@
         <v>23</v>
       </c>
       <c r="F214" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G214" t="s">
         <v>13</v>
@@ -8354,7 +8354,7 @@
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B215" t="s">
         <v>80</v>
@@ -8363,13 +8363,13 @@
         <v>85</v>
       </c>
       <c r="D215" t="s">
-        <v>194</v>
+        <v>87</v>
       </c>
       <c r="E215" t="s">
         <v>23</v>
       </c>
       <c r="F215" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G215" t="s">
         <v>13</v>
@@ -8389,16 +8389,16 @@
         <v>10</v>
       </c>
       <c r="B216" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C216" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D216" t="s">
-        <v>90</v>
+        <v>194</v>
       </c>
       <c r="E216" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F216" t="s">
         <v>15</v>
@@ -8427,7 +8427,7 @@
         <v>89</v>
       </c>
       <c r="D217" t="s">
-        <v>195</v>
+        <v>90</v>
       </c>
       <c r="E217" t="s">
         <v>14</v>
@@ -8450,7 +8450,7 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B218" t="s">
         <v>88</v>
@@ -8482,7 +8482,7 @@
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B219" t="s">
         <v>88</v>
@@ -8514,22 +8514,22 @@
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B220" t="s">
         <v>88</v>
       </c>
       <c r="C220" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D220" t="s">
-        <v>133</v>
+        <v>195</v>
       </c>
       <c r="E220" t="s">
         <v>14</v>
       </c>
       <c r="F220" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G220" t="s">
         <v>13</v>
@@ -8555,13 +8555,13 @@
         <v>91</v>
       </c>
       <c r="D221" t="s">
-        <v>84</v>
+        <v>133</v>
       </c>
       <c r="E221" t="s">
         <v>14</v>
       </c>
       <c r="F221" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G221" t="s">
         <v>13</v>
@@ -8578,7 +8578,7 @@
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>93</v>
+        <v>10</v>
       </c>
       <c r="B222" t="s">
         <v>88</v>
@@ -8610,7 +8610,7 @@
     </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B223" t="s">
         <v>88</v>
@@ -8619,7 +8619,7 @@
         <v>91</v>
       </c>
       <c r="D223" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E223" t="s">
         <v>14</v>
@@ -8651,7 +8651,7 @@
         <v>91</v>
       </c>
       <c r="D224" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E224" t="s">
         <v>14</v>
@@ -8680,10 +8680,10 @@
         <v>88</v>
       </c>
       <c r="C225" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D225" t="s">
-        <v>196</v>
+        <v>87</v>
       </c>
       <c r="E225" t="s">
         <v>14</v>
@@ -8704,14 +8704,46 @@
         <v>13</v>
       </c>
     </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>10</v>
+      </c>
+      <c r="B226" t="s">
+        <v>88</v>
+      </c>
+      <c r="C226" t="s">
+        <v>92</v>
+      </c>
+      <c r="D226" t="s">
+        <v>196</v>
+      </c>
+      <c r="E226" t="s">
+        <v>14</v>
+      </c>
+      <c r="F226" t="s">
+        <v>15</v>
+      </c>
+      <c r="G226" t="s">
+        <v>13</v>
+      </c>
+      <c r="H226" t="s">
+        <v>13</v>
+      </c>
+      <c r="I226" t="s">
+        <v>13</v>
+      </c>
+      <c r="J226" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J225" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J222">
-      <sortCondition ref="B1:B225"/>
+  <autoFilter ref="A1:J226" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J22">
+      <sortCondition ref="D1:D226"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A40:J242">
-    <sortCondition ref="D2:D242"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:J243">
+    <sortCondition ref="D2:D243"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
respiration and CO2 edited to match
</commit_message>
<xml_diff>
--- a/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
+++ b/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesley.atwood\Desktop\GitHub\AgEvidence\AgEvidence_Kenya\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FFFD39-7DC8-4EFD-A74A-F79CC80D2E59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B308CB3E-03FC-462A-89BC-C71225592852}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29025" yWindow="30" windowWidth="28290" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grouplists_Kenya_2021-07-14" sheetId="1" r:id="rId1"/>
@@ -1488,8 +1488,8 @@
   <dimension ref="A1:J226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4:F6"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5329,7 +5329,7 @@
         <v>23</v>
       </c>
       <c r="F120" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="G120" t="s">
         <v>11</v>
@@ -5341,7 +5341,7 @@
         <v>14</v>
       </c>
       <c r="J120" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.35">
@@ -5361,7 +5361,7 @@
         <v>23</v>
       </c>
       <c r="F121" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="G121" t="s">
         <v>11</v>
@@ -5373,7 +5373,7 @@
         <v>14</v>
       </c>
       <c r="J121" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
updated metadata and created KNB files for uploading to repository
</commit_message>
<xml_diff>
--- a/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
+++ b/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesley.atwood\Desktop\GitHub2\AgEvidence\AgEvidence_Kenya\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesley.atwood\Desktop\GitHub\AgEvidence\AgEvidence_Kenya\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91891A18-3364-4909-A9C4-28958A7BB453}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C36CEB4-85EA-40AF-8BF4-351FB3DAF2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="grouplists_Kenya_2021-07-14" sheetId="1" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId1"/>
+    <sheet name="grouplists_Kenya_2021-07-14" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'grouplists_Kenya_2021-07-14'!$A$1:$J$222</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'grouplists_Kenya_2021-07-14'!$A$1:$J$222</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2220" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="206">
   <si>
     <t>Review</t>
   </si>
@@ -616,6 +617,42 @@
   </si>
   <si>
     <t>Phosphorus decomposition rate of buried residues</t>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Name of review</t>
+  </si>
+  <si>
+    <t>Highest grouping level</t>
+  </si>
+  <si>
+    <t>Middle grouping level</t>
+  </si>
+  <si>
+    <t>Finest grouping level</t>
+  </si>
+  <si>
+    <t>Normative interpretation of group_level2 where Negative = assumed societal harm, Positive = assumed societal benefit, and Dependent on other factors</t>
+  </si>
+  <si>
+    <t>Normative interpretation of group_level3 where Negative = assumed societal harm, Positive = assumed societal benefit, and Dependent on other factors</t>
+  </si>
+  <si>
+    <t>Alternate highest grouping level, used when a variable could be classified under more than one grouping</t>
+  </si>
+  <si>
+    <t>Alternate middle grouping level, used when a variable could be classified under more than one grouping</t>
+  </si>
+  <si>
+    <t>Normative interpretation of group_level2_alt where Negative = assumed societal harm, Positive = assumed societal benefit, and Dependent on other factors</t>
+  </si>
+  <si>
+    <t>Normative interpretation of group_level3_alt where Negative = assumed societal harm, Positive = assumed societal benefit, and Dependent on other factors</t>
   </si>
 </sst>
 </file>
@@ -1472,12 +1509,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC0001B-83E3-4DBB-B747-50C6C3430621}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J222"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F224" sqref="F224"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updated with 2010-2020 groups and normative effects
</commit_message>
<xml_diff>
--- a/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
+++ b/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesley.atwood\Desktop\GitHub\AgEvidence\AgEvidence_Kenya\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3537ED9-18CE-4A56-BCBC-D6B004698EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444999EC-82BB-4108-BA10-22E8CC5CB0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32730" yWindow="2835" windowWidth="14400" windowHeight="8265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
-    <sheet name="grouplists_Kenya_2021-07-14" sheetId="1" r:id="rId2"/>
+    <sheet name="grouplists_Kenya" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'grouplists_Kenya_2021-07-14'!$A$1:$J$258</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">grouplists_Kenya!$A$1:$J$261</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2602" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2632" uniqueCount="214">
   <si>
     <t>Review</t>
   </si>
@@ -544,9 +544,6 @@
     <t>Community diversity</t>
   </si>
   <si>
-    <t>Natural enemies</t>
-  </si>
-  <si>
     <t>Natural enemy activity</t>
   </si>
   <si>
@@ -646,34 +643,40 @@
     <t>Costs</t>
   </si>
   <si>
-    <t>Labour Cost</t>
-  </si>
-  <si>
-    <t>Total Cost</t>
-  </si>
-  <si>
-    <t>Variable Cost</t>
-  </si>
-  <si>
     <t>Economic Performance</t>
   </si>
   <si>
-    <t>Benefit Cost Ratio (GRTC)</t>
-  </si>
-  <si>
-    <t>Benefit Cost Ratio (GRVC)</t>
-  </si>
-  <si>
-    <t>Benefit Cost Ratio (NRTC)</t>
-  </si>
-  <si>
-    <t>Gross Margin</t>
-  </si>
-  <si>
-    <t>Gross Return</t>
-  </si>
-  <si>
-    <t>Net Return</t>
+    <t>Benefit cost ratio (GRTC)</t>
+  </si>
+  <si>
+    <t>Benefit cost ratio (GRVC)</t>
+  </si>
+  <si>
+    <t>Benefit cost ratio (NRTC)</t>
+  </si>
+  <si>
+    <t>Labour cost</t>
+  </si>
+  <si>
+    <t>Net return</t>
+  </si>
+  <si>
+    <t>Gross margin</t>
+  </si>
+  <si>
+    <t>Gross return</t>
+  </si>
+  <si>
+    <t>Natural enemy</t>
+  </si>
+  <si>
+    <t>Misc. Micronutrients</t>
+  </si>
+  <si>
+    <t>Total cost</t>
+  </si>
+  <si>
+    <t>Variable cost</t>
   </si>
 </sst>
 </file>
@@ -1544,10 +1547,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" t="s">
         <v>181</v>
-      </c>
-      <c r="B1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1555,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1563,7 +1566,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1571,7 +1574,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1579,7 +1582,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1587,7 +1590,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1595,7 +1598,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1603,7 +1606,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1611,7 +1614,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -1619,7 +1622,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1627,7 +1630,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -1638,11 +1641,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J258"/>
+  <dimension ref="A1:J261"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D105" sqref="D105"/>
+      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D253" sqref="D253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3396,7 +3399,7 @@
         <v>51</v>
       </c>
       <c r="D55" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E55" t="s">
         <v>19</v>
@@ -3428,7 +3431,7 @@
         <v>51</v>
       </c>
       <c r="D56" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E56" t="s">
         <v>19</v>
@@ -3492,7 +3495,7 @@
         <v>51</v>
       </c>
       <c r="D58" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E58" t="s">
         <v>19</v>
@@ -3524,7 +3527,7 @@
         <v>51</v>
       </c>
       <c r="D59" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E59" t="s">
         <v>19</v>
@@ -3652,7 +3655,7 @@
         <v>51</v>
       </c>
       <c r="D63" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
@@ -4449,10 +4452,10 @@
         <v>56</v>
       </c>
       <c r="C88" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D88" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
@@ -4481,10 +4484,10 @@
         <v>56</v>
       </c>
       <c r="C89" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D89" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E89" t="s">
         <v>19</v>
@@ -4513,10 +4516,10 @@
         <v>56</v>
       </c>
       <c r="C90" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D90" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E90" t="s">
         <v>19</v>
@@ -4545,10 +4548,10 @@
         <v>56</v>
       </c>
       <c r="C91" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D91" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E91" t="s">
         <v>19</v>
@@ -4577,10 +4580,10 @@
         <v>56</v>
       </c>
       <c r="C92" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D92" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E92" t="s">
         <v>19</v>
@@ -4609,10 +4612,10 @@
         <v>56</v>
       </c>
       <c r="C93" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D93" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E93" t="s">
         <v>19</v>
@@ -4641,10 +4644,10 @@
         <v>56</v>
       </c>
       <c r="C94" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D94" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E94" t="s">
         <v>19</v>
@@ -4673,10 +4676,10 @@
         <v>56</v>
       </c>
       <c r="C95" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D95" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E95" t="s">
         <v>19</v>
@@ -4705,10 +4708,10 @@
         <v>56</v>
       </c>
       <c r="C96" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D96" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E96" t="s">
         <v>19</v>
@@ -4737,10 +4740,10 @@
         <v>56</v>
       </c>
       <c r="C97" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D97" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E97" t="s">
         <v>14</v>
@@ -4769,10 +4772,10 @@
         <v>56</v>
       </c>
       <c r="C98" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D98" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E98" t="s">
         <v>14</v>
@@ -4801,10 +4804,10 @@
         <v>56</v>
       </c>
       <c r="C99" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D99" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E99" t="s">
         <v>14</v>
@@ -4836,7 +4839,7 @@
         <v>57</v>
       </c>
       <c r="D100" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E100" t="s">
         <v>19</v>
@@ -4868,7 +4871,7 @@
         <v>57</v>
       </c>
       <c r="D101" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E101" t="s">
         <v>19</v>
@@ -4900,7 +4903,7 @@
         <v>57</v>
       </c>
       <c r="D102" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E102" t="s">
         <v>19</v>
@@ -4932,7 +4935,7 @@
         <v>57</v>
       </c>
       <c r="D103" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E103" t="s">
         <v>19</v>
@@ -4964,7 +4967,7 @@
         <v>57</v>
       </c>
       <c r="D104" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E104" t="s">
         <v>19</v>
@@ -4996,7 +4999,7 @@
         <v>57</v>
       </c>
       <c r="D105" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E105" t="s">
         <v>19</v>
@@ -5028,7 +5031,7 @@
         <v>57</v>
       </c>
       <c r="D106" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E106" t="s">
         <v>19</v>
@@ -5060,7 +5063,7 @@
         <v>57</v>
       </c>
       <c r="D107" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E107" t="s">
         <v>19</v>
@@ -5092,7 +5095,7 @@
         <v>57</v>
       </c>
       <c r="D108" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E108" t="s">
         <v>19</v>
@@ -5700,7 +5703,7 @@
         <v>60</v>
       </c>
       <c r="D127" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E127" t="s">
         <v>23</v>
@@ -5732,7 +5735,7 @@
         <v>60</v>
       </c>
       <c r="D128" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E128" t="s">
         <v>23</v>
@@ -5956,7 +5959,7 @@
         <v>21</v>
       </c>
       <c r="D135" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E135" t="s">
         <v>23</v>
@@ -7716,7 +7719,7 @@
         <v>74</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
       <c r="E190" s="3" t="s">
         <v>19</v>
@@ -7748,7 +7751,7 @@
         <v>74</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
       <c r="E191" t="s">
         <v>19</v>
@@ -7780,7 +7783,7 @@
         <v>74</v>
       </c>
       <c r="D192" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E192" t="s">
         <v>19</v>
@@ -7972,7 +7975,7 @@
         <v>75</v>
       </c>
       <c r="D198" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E198" t="s">
         <v>14</v>
@@ -8004,7 +8007,7 @@
         <v>75</v>
       </c>
       <c r="D199" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E199" t="s">
         <v>14</v>
@@ -8036,7 +8039,7 @@
         <v>75</v>
       </c>
       <c r="D200" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E200" t="s">
         <v>14</v>
@@ -8196,7 +8199,7 @@
         <v>108</v>
       </c>
       <c r="D205" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E205" t="s">
         <v>19</v>
@@ -8228,7 +8231,7 @@
         <v>108</v>
       </c>
       <c r="D206" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E206" t="s">
         <v>19</v>
@@ -8260,7 +8263,7 @@
         <v>108</v>
       </c>
       <c r="D207" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E207" t="s">
         <v>19</v>
@@ -8289,16 +8292,16 @@
         <v>78</v>
       </c>
       <c r="C208" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="D208" t="s">
-        <v>79</v>
+        <v>211</v>
       </c>
       <c r="E208" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F208" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G208" t="s">
         <v>13</v>
@@ -8315,22 +8318,22 @@
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B209" t="s">
         <v>78</v>
       </c>
       <c r="C209" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="D209" t="s">
-        <v>79</v>
+        <v>211</v>
       </c>
       <c r="E209" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F209" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G209" t="s">
         <v>13</v>
@@ -8347,22 +8350,22 @@
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B210" t="s">
         <v>78</v>
       </c>
       <c r="C210" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="D210" t="s">
-        <v>128</v>
+        <v>211</v>
       </c>
       <c r="E210" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F210" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G210" t="s">
         <v>13</v>
@@ -8379,7 +8382,7 @@
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B211" t="s">
         <v>78</v>
@@ -8388,7 +8391,7 @@
         <v>82</v>
       </c>
       <c r="D211" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="E211" t="s">
         <v>23</v>
@@ -8420,7 +8423,7 @@
         <v>82</v>
       </c>
       <c r="D212" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="E212" t="s">
         <v>23</v>
@@ -8452,7 +8455,7 @@
         <v>82</v>
       </c>
       <c r="D213" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="E213" t="s">
         <v>23</v>
@@ -8475,7 +8478,7 @@
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B214" t="s">
         <v>78</v>
@@ -8484,7 +8487,7 @@
         <v>82</v>
       </c>
       <c r="D214" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="E214" t="s">
         <v>23</v>
@@ -8507,7 +8510,7 @@
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B215" t="s">
         <v>78</v>
@@ -8516,13 +8519,13 @@
         <v>82</v>
       </c>
       <c r="D215" t="s">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="E215" t="s">
         <v>23</v>
       </c>
       <c r="F215" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G215" t="s">
         <v>13</v>
@@ -8539,7 +8542,7 @@
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B216" t="s">
         <v>78</v>
@@ -8548,7 +8551,7 @@
         <v>82</v>
       </c>
       <c r="D216" t="s">
-        <v>175</v>
+        <v>81</v>
       </c>
       <c r="E216" t="s">
         <v>23</v>
@@ -8571,7 +8574,7 @@
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B217" t="s">
         <v>78</v>
@@ -8580,7 +8583,7 @@
         <v>82</v>
       </c>
       <c r="D217" t="s">
-        <v>175</v>
+        <v>81</v>
       </c>
       <c r="E217" t="s">
         <v>23</v>
@@ -8603,7 +8606,7 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B218" t="s">
         <v>78</v>
@@ -8612,13 +8615,13 @@
         <v>82</v>
       </c>
       <c r="D218" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E218" t="s">
         <v>23</v>
       </c>
       <c r="F218" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G218" t="s">
         <v>13</v>
@@ -8641,10 +8644,10 @@
         <v>78</v>
       </c>
       <c r="C219" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D219" t="s">
-        <v>84</v>
+        <v>174</v>
       </c>
       <c r="E219" t="s">
         <v>23</v>
@@ -8673,10 +8676,10 @@
         <v>78</v>
       </c>
       <c r="C220" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D220" t="s">
-        <v>84</v>
+        <v>174</v>
       </c>
       <c r="E220" t="s">
         <v>23</v>
@@ -8705,10 +8708,10 @@
         <v>78</v>
       </c>
       <c r="C221" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D221" t="s">
-        <v>84</v>
+        <v>174</v>
       </c>
       <c r="E221" t="s">
         <v>23</v>
@@ -8740,13 +8743,13 @@
         <v>83</v>
       </c>
       <c r="D222" t="s">
-        <v>176</v>
+        <v>84</v>
       </c>
       <c r="E222" t="s">
         <v>23</v>
       </c>
       <c r="F222" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G222" t="s">
         <v>13</v>
@@ -8763,7 +8766,7 @@
     </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B223" t="s">
         <v>78</v>
@@ -8772,13 +8775,13 @@
         <v>83</v>
       </c>
       <c r="D223" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E223" t="s">
         <v>23</v>
       </c>
       <c r="F223" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G223" t="s">
         <v>13</v>
@@ -8795,7 +8798,7 @@
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B224" t="s">
         <v>78</v>
@@ -8804,7 +8807,7 @@
         <v>83</v>
       </c>
       <c r="D224" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E224" t="s">
         <v>23</v>
@@ -8827,7 +8830,7 @@
     </row>
     <row r="225" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B225" t="s">
         <v>78</v>
@@ -8836,13 +8839,13 @@
         <v>83</v>
       </c>
       <c r="D225" t="s">
-        <v>85</v>
+        <v>175</v>
       </c>
       <c r="E225" t="s">
         <v>23</v>
       </c>
       <c r="F225" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G225" t="s">
         <v>13</v>
@@ -8868,13 +8871,13 @@
         <v>83</v>
       </c>
       <c r="D226" t="s">
-        <v>177</v>
+        <v>85</v>
       </c>
       <c r="E226" t="s">
         <v>23</v>
       </c>
       <c r="F226" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G226" t="s">
         <v>13</v>
@@ -8891,22 +8894,22 @@
     </row>
     <row r="227" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B227" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C227" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D227" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E227" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F227" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G227" t="s">
         <v>13</v>
@@ -8923,22 +8926,22 @@
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B228" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C228" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D228" t="s">
-        <v>178</v>
+        <v>85</v>
       </c>
       <c r="E228" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F228" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G228" t="s">
         <v>13</v>
@@ -8955,19 +8958,19 @@
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B229" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C229" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D229" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E229" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F229" t="s">
         <v>15</v>
@@ -8987,7 +8990,7 @@
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B230" t="s">
         <v>86</v>
@@ -8996,7 +8999,7 @@
         <v>87</v>
       </c>
       <c r="D230" t="s">
-        <v>178</v>
+        <v>88</v>
       </c>
       <c r="E230" t="s">
         <v>14</v>
@@ -9025,16 +9028,16 @@
         <v>86</v>
       </c>
       <c r="C231" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D231" t="s">
-        <v>128</v>
+        <v>177</v>
       </c>
       <c r="E231" t="s">
         <v>14</v>
       </c>
       <c r="F231" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G231" t="s">
         <v>13</v>
@@ -9051,16 +9054,16 @@
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B232" t="s">
         <v>86</v>
       </c>
       <c r="C232" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D232" t="s">
-        <v>82</v>
+        <v>177</v>
       </c>
       <c r="E232" t="s">
         <v>14</v>
@@ -9089,10 +9092,10 @@
         <v>86</v>
       </c>
       <c r="C233" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D233" t="s">
-        <v>82</v>
+        <v>177</v>
       </c>
       <c r="E233" t="s">
         <v>14</v>
@@ -9124,13 +9127,13 @@
         <v>89</v>
       </c>
       <c r="D234" t="s">
-        <v>84</v>
+        <v>128</v>
       </c>
       <c r="E234" t="s">
         <v>14</v>
       </c>
       <c r="F234" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G234" t="s">
         <v>13</v>
@@ -9156,7 +9159,7 @@
         <v>89</v>
       </c>
       <c r="D235" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E235" t="s">
         <v>14</v>
@@ -9179,16 +9182,16 @@
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B236" t="s">
         <v>86</v>
       </c>
       <c r="C236" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D236" t="s">
-        <v>179</v>
+        <v>82</v>
       </c>
       <c r="E236" t="s">
         <v>14</v>
@@ -9211,16 +9214,16 @@
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B237" t="s">
         <v>86</v>
       </c>
       <c r="C237" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D237" t="s">
-        <v>179</v>
+        <v>84</v>
       </c>
       <c r="E237" t="s">
         <v>14</v>
@@ -9243,7 +9246,7 @@
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B238" t="s">
         <v>86</v>
@@ -9252,7 +9255,7 @@
         <v>89</v>
       </c>
       <c r="D238" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E238" t="s">
         <v>14</v>
@@ -9275,16 +9278,16 @@
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B239" t="s">
         <v>86</v>
       </c>
       <c r="C239" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D239" t="s">
-        <v>84</v>
+        <v>178</v>
       </c>
       <c r="E239" t="s">
         <v>14</v>
@@ -9313,16 +9316,16 @@
         <v>86</v>
       </c>
       <c r="C240" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D240" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="E240" t="s">
         <v>14</v>
       </c>
       <c r="F240" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G240" t="s">
         <v>13</v>
@@ -9342,16 +9345,16 @@
         <v>16</v>
       </c>
       <c r="B241" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="C241" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="D241" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E241" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F241" t="s">
         <v>15</v>
@@ -9374,19 +9377,19 @@
         <v>16</v>
       </c>
       <c r="B242" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="C242" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="D242" t="s">
-        <v>196</v>
+        <v>84</v>
       </c>
       <c r="E242" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F242" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G242" t="s">
         <v>13</v>
@@ -9403,22 +9406,22 @@
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B243" t="s">
-        <v>26</v>
-      </c>
-      <c r="C243" s="2" t="s">
-        <v>55</v>
+        <v>86</v>
+      </c>
+      <c r="C243" t="s">
+        <v>89</v>
       </c>
       <c r="D243" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E243" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F243" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G243" t="s">
         <v>13</v>
@@ -9438,16 +9441,16 @@
         <v>16</v>
       </c>
       <c r="B244" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="C244" t="s">
-        <v>202</v>
+        <v>63</v>
       </c>
       <c r="D244" t="s">
-        <v>204</v>
+        <v>65</v>
       </c>
       <c r="E244" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F244" t="s">
         <v>15</v>
@@ -9467,22 +9470,22 @@
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B245" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="C245" t="s">
-        <v>202</v>
+        <v>63</v>
       </c>
       <c r="D245" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E245" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F245" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G245" t="s">
         <v>13</v>
@@ -9499,97 +9502,97 @@
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B246" t="s">
+        <v>26</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D246" t="s">
+        <v>197</v>
+      </c>
+      <c r="E246" t="s">
+        <v>19</v>
+      </c>
+      <c r="F246" t="s">
+        <v>22</v>
+      </c>
+      <c r="G246" t="s">
+        <v>13</v>
+      </c>
+      <c r="H246" t="s">
+        <v>13</v>
+      </c>
+      <c r="I246" t="s">
+        <v>13</v>
+      </c>
+      <c r="J246" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A247" t="s">
+        <v>16</v>
+      </c>
+      <c r="B247" t="s">
         <v>56</v>
       </c>
-      <c r="C246" t="s">
-        <v>202</v>
-      </c>
-      <c r="D246" t="s">
-        <v>204</v>
-      </c>
-      <c r="E246" t="s">
+      <c r="C247" t="s">
+        <v>201</v>
+      </c>
+      <c r="D247" t="s">
+        <v>212</v>
+      </c>
+      <c r="E247" t="s">
         <v>14</v>
       </c>
-      <c r="F246" t="s">
+      <c r="F247" t="s">
         <v>15</v>
       </c>
-      <c r="G246" t="s">
-        <v>13</v>
-      </c>
-      <c r="H246" t="s">
-        <v>13</v>
-      </c>
-      <c r="I246" t="s">
-        <v>13</v>
-      </c>
-      <c r="J246" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A247" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B247" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C247" t="s">
-        <v>202</v>
-      </c>
-      <c r="D247" t="s">
-        <v>205</v>
-      </c>
-      <c r="E247" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F247" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G247" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H247" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I247" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J247" s="3" t="s">
+      <c r="G247" t="s">
+        <v>13</v>
+      </c>
+      <c r="H247" t="s">
+        <v>13</v>
+      </c>
+      <c r="I247" t="s">
+        <v>13</v>
+      </c>
+      <c r="J247" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>16</v>
-      </c>
-      <c r="B248" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B248" t="s">
         <v>56</v>
       </c>
       <c r="C248" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D248" t="s">
-        <v>205</v>
-      </c>
-      <c r="E248" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E248" t="s">
         <v>14</v>
       </c>
-      <c r="F248" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G248" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H248" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I248" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J248" s="3" t="s">
+      <c r="F248" t="s">
+        <v>15</v>
+      </c>
+      <c r="G248" t="s">
+        <v>13</v>
+      </c>
+      <c r="H248" t="s">
+        <v>13</v>
+      </c>
+      <c r="I248" t="s">
+        <v>13</v>
+      </c>
+      <c r="J248" t="s">
         <v>13</v>
       </c>
     </row>
@@ -9597,95 +9600,95 @@
       <c r="A249" t="s">
         <v>10</v>
       </c>
-      <c r="B249" s="3" t="s">
+      <c r="B249" t="s">
         <v>56</v>
       </c>
       <c r="C249" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D249" t="s">
-        <v>205</v>
-      </c>
-      <c r="E249" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E249" t="s">
         <v>14</v>
       </c>
-      <c r="F249" s="3" t="s">
+      <c r="F249" t="s">
+        <v>15</v>
+      </c>
+      <c r="G249" t="s">
+        <v>13</v>
+      </c>
+      <c r="H249" t="s">
+        <v>13</v>
+      </c>
+      <c r="I249" t="s">
+        <v>13</v>
+      </c>
+      <c r="J249" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A250" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B250" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C250" t="s">
+        <v>201</v>
+      </c>
+      <c r="D250" t="s">
+        <v>213</v>
+      </c>
+      <c r="E250" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F250" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G249" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H249" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I249" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J249" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A250" t="s">
-        <v>10</v>
-      </c>
-      <c r="B250" t="s">
-        <v>20</v>
-      </c>
-      <c r="C250" t="s">
-        <v>63</v>
-      </c>
-      <c r="D250" t="s">
-        <v>196</v>
-      </c>
-      <c r="E250" t="s">
-        <v>23</v>
-      </c>
-      <c r="F250" t="s">
-        <v>22</v>
-      </c>
-      <c r="G250" t="s">
-        <v>13</v>
-      </c>
-      <c r="H250" t="s">
-        <v>13</v>
-      </c>
-      <c r="I250" t="s">
-        <v>13</v>
-      </c>
-      <c r="J250" t="s">
+      <c r="G250" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H250" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I250" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J250" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>10</v>
-      </c>
-      <c r="B251" t="s">
-        <v>26</v>
-      </c>
-      <c r="C251" s="2" t="s">
-        <v>55</v>
+        <v>16</v>
+      </c>
+      <c r="B251" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C251" t="s">
+        <v>201</v>
       </c>
       <c r="D251" t="s">
-        <v>47</v>
-      </c>
-      <c r="E251" t="s">
-        <v>19</v>
-      </c>
-      <c r="F251" t="s">
-        <v>22</v>
-      </c>
-      <c r="G251" t="s">
-        <v>13</v>
-      </c>
-      <c r="H251" t="s">
-        <v>13</v>
-      </c>
-      <c r="I251" t="s">
-        <v>13</v>
-      </c>
-      <c r="J251" t="s">
+        <v>213</v>
+      </c>
+      <c r="E251" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F251" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G251" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H251" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I251" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J251" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -9693,52 +9696,52 @@
       <c r="A252" t="s">
         <v>10</v>
       </c>
-      <c r="B252" t="s">
-        <v>26</v>
+      <c r="B252" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C252" t="s">
-        <v>30</v>
+        <v>201</v>
       </c>
       <c r="D252" t="s">
-        <v>124</v>
-      </c>
-      <c r="E252" t="s">
-        <v>19</v>
-      </c>
-      <c r="F252" t="s">
-        <v>22</v>
-      </c>
-      <c r="G252" t="s">
-        <v>13</v>
-      </c>
-      <c r="H252" t="s">
-        <v>13</v>
-      </c>
-      <c r="I252" t="s">
-        <v>13</v>
-      </c>
-      <c r="J252" t="s">
+        <v>213</v>
+      </c>
+      <c r="E252" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F252" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G252" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H252" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I252" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J252" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A253" s="3" t="s">
-        <v>91</v>
+      <c r="A253" t="s">
+        <v>10</v>
       </c>
       <c r="B253" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C253" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D253" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="E253" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F253" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G253" t="s">
         <v>13</v>
@@ -9755,22 +9758,22 @@
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B254" t="s">
-        <v>20</v>
-      </c>
-      <c r="C254" t="s">
-        <v>63</v>
+        <v>26</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D254" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
       <c r="E254" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F254" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G254" t="s">
         <v>13</v>
@@ -9793,48 +9796,48 @@
         <v>26</v>
       </c>
       <c r="C255" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D255" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E255" t="s">
+        <v>19</v>
+      </c>
+      <c r="F255" t="s">
+        <v>22</v>
+      </c>
+      <c r="G255" t="s">
+        <v>13</v>
+      </c>
+      <c r="H255" t="s">
+        <v>13</v>
+      </c>
+      <c r="I255" t="s">
+        <v>13</v>
+      </c>
+      <c r="J255" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A256" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B256" t="s">
+        <v>28</v>
+      </c>
+      <c r="C256" t="s">
+        <v>75</v>
+      </c>
+      <c r="D256" t="s">
+        <v>170</v>
+      </c>
+      <c r="E256" t="s">
         <v>14</v>
       </c>
-      <c r="F255" t="s">
+      <c r="F256" t="s">
         <v>15</v>
-      </c>
-      <c r="G255" t="s">
-        <v>28</v>
-      </c>
-      <c r="H255" t="s">
-        <v>29</v>
-      </c>
-      <c r="I255" t="s">
-        <v>14</v>
-      </c>
-      <c r="J255" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A256" t="s">
-        <v>91</v>
-      </c>
-      <c r="B256" t="s">
-        <v>20</v>
-      </c>
-      <c r="C256" t="s">
-        <v>60</v>
-      </c>
-      <c r="D256" t="s">
-        <v>200</v>
-      </c>
-      <c r="E256" t="s">
-        <v>23</v>
-      </c>
-      <c r="F256" t="s">
-        <v>22</v>
       </c>
       <c r="G256" t="s">
         <v>13</v>
@@ -9857,70 +9860,166 @@
         <v>20</v>
       </c>
       <c r="C257" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D257" t="s">
-        <v>92</v>
+        <v>149</v>
       </c>
       <c r="E257" t="s">
         <v>23</v>
       </c>
       <c r="F257" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="G257" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H257" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I257" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J257" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="258" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B258" t="s">
         <v>26</v>
       </c>
       <c r="C258" t="s">
+        <v>27</v>
+      </c>
+      <c r="D258" t="s">
+        <v>120</v>
+      </c>
+      <c r="E258" t="s">
+        <v>14</v>
+      </c>
+      <c r="F258" t="s">
+        <v>15</v>
+      </c>
+      <c r="G258" t="s">
+        <v>28</v>
+      </c>
+      <c r="H258" t="s">
+        <v>29</v>
+      </c>
+      <c r="I258" t="s">
+        <v>14</v>
+      </c>
+      <c r="J258" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
+        <v>91</v>
+      </c>
+      <c r="B259" t="s">
+        <v>20</v>
+      </c>
+      <c r="C259" t="s">
+        <v>60</v>
+      </c>
+      <c r="D259" t="s">
+        <v>199</v>
+      </c>
+      <c r="E259" t="s">
+        <v>23</v>
+      </c>
+      <c r="F259" t="s">
+        <v>22</v>
+      </c>
+      <c r="G259" t="s">
+        <v>13</v>
+      </c>
+      <c r="H259" t="s">
+        <v>13</v>
+      </c>
+      <c r="I259" t="s">
+        <v>13</v>
+      </c>
+      <c r="J259" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
+        <v>91</v>
+      </c>
+      <c r="B260" t="s">
+        <v>20</v>
+      </c>
+      <c r="C260" t="s">
+        <v>60</v>
+      </c>
+      <c r="D260" t="s">
+        <v>92</v>
+      </c>
+      <c r="E260" t="s">
+        <v>23</v>
+      </c>
+      <c r="F260" t="s">
+        <v>14</v>
+      </c>
+      <c r="G260" t="s">
+        <v>11</v>
+      </c>
+      <c r="H260" t="s">
+        <v>12</v>
+      </c>
+      <c r="I260" t="s">
+        <v>14</v>
+      </c>
+      <c r="J260" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
+        <v>91</v>
+      </c>
+      <c r="B261" t="s">
+        <v>26</v>
+      </c>
+      <c r="C261" t="s">
         <v>30</v>
       </c>
-      <c r="D258" t="s">
-        <v>201</v>
-      </c>
-      <c r="E258" t="s">
-        <v>19</v>
-      </c>
-      <c r="F258" t="s">
-        <v>22</v>
-      </c>
-      <c r="G258" t="s">
-        <v>13</v>
-      </c>
-      <c r="H258" t="s">
-        <v>13</v>
-      </c>
-      <c r="I258" t="s">
-        <v>13</v>
-      </c>
-      <c r="J258" t="s">
+      <c r="D261" t="s">
+        <v>200</v>
+      </c>
+      <c r="E261" t="s">
+        <v>19</v>
+      </c>
+      <c r="F261" t="s">
+        <v>22</v>
+      </c>
+      <c r="G261" t="s">
+        <v>13</v>
+      </c>
+      <c r="H261" t="s">
+        <v>13</v>
+      </c>
+      <c r="I261" t="s">
+        <v>13</v>
+      </c>
+      <c r="J261" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J258" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:J255">
-      <sortCondition ref="D1:D257"/>
+  <autoFilter ref="A1:J261" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:J258">
+      <sortCondition ref="D1:D260"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:J250">
-    <sortCondition ref="D2:D250"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:J253">
+    <sortCondition ref="D2:D253"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
data errors corrected, normative group added
</commit_message>
<xml_diff>
--- a/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
+++ b/AgEvidence_Kenya/data/normative-effects-Kenya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesley.atwood\Desktop\GitHub\AgEvidence\AgEvidence_Kenya\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1930BAA-39F8-402D-AF45-44252DE64AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269C422B-A161-4FEF-A5D5-5033C24364CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="grouplists_Kenya" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">grouplists_Kenya!$A$1:$J$261</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">grouplists_Kenya!$A$1:$J$262</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2632" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="214">
   <si>
     <t>Review</t>
   </si>
@@ -1641,11 +1641,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J261"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:J262"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C263" sqref="C263"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1692,7 +1693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1724,7 +1725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -1756,7 +1757,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1788,7 +1789,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1820,7 +1821,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -1852,7 +1853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1884,7 +1885,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1916,7 +1917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1948,7 +1949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1980,7 +1981,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>91</v>
       </c>
@@ -2012,7 +2013,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -2044,7 +2045,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -2076,7 +2077,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2108,7 +2109,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2140,7 +2141,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -2172,7 +2173,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2204,7 +2205,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -2236,7 +2237,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -2268,7 +2269,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -2300,7 +2301,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -2332,7 +2333,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -2364,7 +2365,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2396,7 +2397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>91</v>
       </c>
@@ -2428,7 +2429,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -2460,7 +2461,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2492,7 +2493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>91</v>
       </c>
@@ -2524,7 +2525,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2556,7 +2557,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -2588,7 +2589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -2620,7 +2621,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2652,7 +2653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>91</v>
       </c>
@@ -2684,7 +2685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2716,7 +2717,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2748,7 +2749,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2780,7 +2781,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2812,7 +2813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -2844,7 +2845,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2876,7 +2877,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>91</v>
       </c>
@@ -2908,7 +2909,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -2940,7 +2941,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>91</v>
       </c>
@@ -2972,7 +2973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -3004,7 +3005,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>91</v>
       </c>
@@ -3036,7 +3037,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -3068,7 +3069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -3100,7 +3101,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -3132,7 +3133,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -3164,7 +3165,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -3196,7 +3197,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -3228,7 +3229,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -3260,7 +3261,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -3292,7 +3293,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -3324,7 +3325,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>91</v>
       </c>
@@ -3356,7 +3357,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -3388,7 +3389,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -3420,7 +3421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>91</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>91</v>
       </c>
@@ -3484,7 +3485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -3516,7 +3517,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -3548,7 +3549,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -3580,7 +3581,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -3612,7 +3613,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>91</v>
       </c>
@@ -3644,7 +3645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>91</v>
       </c>
@@ -3676,7 +3677,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -3708,7 +3709,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>91</v>
       </c>
@@ -3740,7 +3741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -3772,7 +3773,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -3804,7 +3805,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -3836,7 +3837,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -3868,7 +3869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -3900,7 +3901,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>91</v>
       </c>
@@ -3932,7 +3933,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>16</v>
       </c>
@@ -3964,7 +3965,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -3996,7 +3997,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -4028,7 +4029,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -4060,7 +4061,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -4092,7 +4093,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -4124,7 +4125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>91</v>
       </c>
@@ -4156,7 +4157,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>16</v>
       </c>
@@ -4188,7 +4189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -4220,7 +4221,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -4252,7 +4253,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>91</v>
       </c>
@@ -4284,7 +4285,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>10</v>
       </c>
@@ -4316,7 +4317,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -4348,7 +4349,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -4380,7 +4381,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -4412,7 +4413,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>10</v>
       </c>
@@ -4444,7 +4445,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -4476,7 +4477,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>16</v>
       </c>
@@ -4508,7 +4509,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>10</v>
       </c>
@@ -4540,7 +4541,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -4572,7 +4573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -4604,7 +4605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>10</v>
       </c>
@@ -4636,7 +4637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>91</v>
       </c>
@@ -4668,7 +4669,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>16</v>
       </c>
@@ -4700,7 +4701,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>10</v>
       </c>
@@ -4732,7 +4733,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>16</v>
       </c>
@@ -4764,7 +4765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>91</v>
       </c>
@@ -4796,7 +4797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>10</v>
       </c>
@@ -4828,7 +4829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -4860,7 +4861,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>10</v>
       </c>
@@ -4892,7 +4893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>91</v>
       </c>
@@ -4924,7 +4925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>16</v>
       </c>
@@ -4956,7 +4957,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>10</v>
       </c>
@@ -4988,7 +4989,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
         <v>91</v>
       </c>
@@ -5020,7 +5021,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>16</v>
       </c>
@@ -5052,7 +5053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>91</v>
       </c>
@@ -5084,7 +5085,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>10</v>
       </c>
@@ -5630,7 +5631,7 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B125" t="s">
         <v>20</v>
@@ -5639,13 +5640,13 @@
         <v>60</v>
       </c>
       <c r="D125" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E125" t="s">
         <v>23</v>
       </c>
       <c r="F125" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G125" t="s">
         <v>13</v>
@@ -5662,7 +5663,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B126" t="s">
         <v>20</v>
@@ -5694,7 +5695,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B127" t="s">
         <v>20</v>
@@ -5703,7 +5704,7 @@
         <v>60</v>
       </c>
       <c r="D127" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="E127" t="s">
         <v>23</v>
@@ -5726,7 +5727,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B128" t="s">
         <v>20</v>
@@ -5758,7 +5759,7 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B129" t="s">
         <v>20</v>
@@ -5767,30 +5768,30 @@
         <v>60</v>
       </c>
       <c r="D129" t="s">
-        <v>92</v>
+        <v>179</v>
       </c>
       <c r="E129" t="s">
         <v>23</v>
       </c>
       <c r="F129" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="G129" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H129" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I129" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J129" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B130" t="s">
         <v>20</v>
@@ -5822,34 +5823,34 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B131" t="s">
         <v>20</v>
       </c>
       <c r="C131" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="D131" t="s">
-        <v>145</v>
+        <v>92</v>
       </c>
       <c r="E131" t="s">
         <v>23</v>
       </c>
       <c r="F131" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G131" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H131" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.35">
@@ -5863,7 +5864,7 @@
         <v>21</v>
       </c>
       <c r="D132" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E132" t="s">
         <v>23</v>
@@ -5872,16 +5873,16 @@
         <v>22</v>
       </c>
       <c r="G132" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H132" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I132" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J132" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.35">
@@ -5895,7 +5896,7 @@
         <v>21</v>
       </c>
       <c r="D133" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E133" t="s">
         <v>23</v>
@@ -5904,21 +5905,21 @@
         <v>22</v>
       </c>
       <c r="G133" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H133" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I133" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J133" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B134" t="s">
         <v>20</v>
@@ -5927,13 +5928,13 @@
         <v>21</v>
       </c>
       <c r="D134" t="s">
-        <v>62</v>
+        <v>147</v>
       </c>
       <c r="E134" t="s">
         <v>23</v>
       </c>
       <c r="F134" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G134" t="s">
         <v>13</v>
@@ -5950,7 +5951,7 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B135" t="s">
         <v>20</v>
@@ -5959,7 +5960,7 @@
         <v>21</v>
       </c>
       <c r="D135" t="s">
-        <v>198</v>
+        <v>62</v>
       </c>
       <c r="E135" t="s">
         <v>23</v>
@@ -5991,7 +5992,7 @@
         <v>21</v>
       </c>
       <c r="D136" t="s">
-        <v>62</v>
+        <v>198</v>
       </c>
       <c r="E136" t="s">
         <v>23</v>
@@ -6014,7 +6015,7 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B137" t="s">
         <v>20</v>
@@ -6046,7 +6047,7 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B138" t="s">
         <v>20</v>
@@ -6055,30 +6056,30 @@
         <v>21</v>
       </c>
       <c r="D138" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="E138" t="s">
         <v>23</v>
       </c>
       <c r="F138" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G138" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H138" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I138" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J138" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B139" t="s">
         <v>20</v>
@@ -6087,7 +6088,7 @@
         <v>21</v>
       </c>
       <c r="D139" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="E139" t="s">
         <v>23</v>
@@ -6110,7 +6111,7 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B140" t="s">
         <v>20</v>
@@ -6142,7 +6143,7 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B141" t="s">
         <v>20</v>
@@ -6174,39 +6175,39 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B142" t="s">
         <v>20</v>
       </c>
       <c r="C142" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="D142" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E142" t="s">
         <v>23</v>
       </c>
       <c r="F142" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G142" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H142" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I142" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J142" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B143" t="s">
         <v>20</v>
@@ -6215,13 +6216,13 @@
         <v>63</v>
       </c>
       <c r="D143" t="s">
-        <v>65</v>
+        <v>149</v>
       </c>
       <c r="E143" t="s">
         <v>23</v>
       </c>
       <c r="F143" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G143" t="s">
         <v>13</v>
@@ -6238,7 +6239,7 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B144" t="s">
         <v>20</v>
@@ -6247,7 +6248,7 @@
         <v>63</v>
       </c>
       <c r="D144" t="s">
-        <v>150</v>
+        <v>65</v>
       </c>
       <c r="E144" t="s">
         <v>23</v>
@@ -6256,21 +6257,21 @@
         <v>15</v>
       </c>
       <c r="G144" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H144" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="I144" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J144" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B145" t="s">
         <v>20</v>
@@ -6288,21 +6289,21 @@
         <v>15</v>
       </c>
       <c r="G145" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H145" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="I145" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J145" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B146" t="s">
         <v>20</v>
@@ -6343,13 +6344,13 @@
         <v>63</v>
       </c>
       <c r="D147" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E147" t="s">
         <v>23</v>
       </c>
       <c r="F147" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G147" t="s">
         <v>13</v>
@@ -6366,7 +6367,7 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B148" t="s">
         <v>20</v>
@@ -6404,13 +6405,13 @@
         <v>20</v>
       </c>
       <c r="C149" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D149" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E149" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F149" t="s">
         <v>22</v>
@@ -6430,7 +6431,7 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B150" t="s">
         <v>20</v>
@@ -6462,7 +6463,7 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B151" t="s">
         <v>20</v>
@@ -6494,7 +6495,7 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B152" t="s">
         <v>20</v>
@@ -6503,7 +6504,7 @@
         <v>64</v>
       </c>
       <c r="D152" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E152" t="s">
         <v>19</v>
@@ -6526,7 +6527,7 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B153" t="s">
         <v>20</v>
@@ -6558,22 +6559,22 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B154" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C154" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="D154" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="E154" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F154" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G154" t="s">
         <v>13</v>
@@ -6588,7 +6589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>10</v>
       </c>
@@ -6596,10 +6597,10 @@
         <v>28</v>
       </c>
       <c r="C155" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="D155" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
       <c r="E155" t="s">
         <v>14</v>
@@ -6608,19 +6609,19 @@
         <v>15</v>
       </c>
       <c r="G155" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="H155" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="I155" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J155" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>10</v>
       </c>
@@ -6631,7 +6632,7 @@
         <v>27</v>
       </c>
       <c r="D156" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E156" t="s">
         <v>14</v>
@@ -6652,7 +6653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>10</v>
       </c>
@@ -6663,7 +6664,7 @@
         <v>27</v>
       </c>
       <c r="D157" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E157" t="s">
         <v>14</v>
@@ -6684,7 +6685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>10</v>
       </c>
@@ -6695,7 +6696,7 @@
         <v>27</v>
       </c>
       <c r="D158" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E158" t="s">
         <v>14</v>
@@ -6716,7 +6717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>10</v>
       </c>
@@ -6727,7 +6728,7 @@
         <v>27</v>
       </c>
       <c r="D159" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E159" t="s">
         <v>14</v>
@@ -6748,9 +6749,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B160" t="s">
         <v>28</v>
@@ -6759,7 +6760,7 @@
         <v>27</v>
       </c>
       <c r="D160" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E160" t="s">
         <v>14</v>
@@ -6780,18 +6781,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B161" t="s">
         <v>28</v>
       </c>
       <c r="C161" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D161" t="s">
-        <v>66</v>
+        <v>159</v>
       </c>
       <c r="E161" t="s">
         <v>14</v>
@@ -6800,19 +6801,19 @@
         <v>15</v>
       </c>
       <c r="G161" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="H161" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="I161" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J161" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>10</v>
       </c>
@@ -6823,7 +6824,7 @@
         <v>29</v>
       </c>
       <c r="D162" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="E162" t="s">
         <v>14</v>
@@ -6844,7 +6845,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>10</v>
       </c>
@@ -6855,7 +6856,7 @@
         <v>29</v>
       </c>
       <c r="D163" t="s">
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="E163" t="s">
         <v>14</v>
@@ -6876,7 +6877,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>10</v>
       </c>
@@ -6887,7 +6888,7 @@
         <v>29</v>
       </c>
       <c r="D164" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E164" t="s">
         <v>14</v>
@@ -6908,7 +6909,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>10</v>
       </c>
@@ -6919,7 +6920,7 @@
         <v>29</v>
       </c>
       <c r="D165" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E165" t="s">
         <v>14</v>
@@ -6940,9 +6941,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B166" t="s">
         <v>28</v>
@@ -6951,7 +6952,7 @@
         <v>29</v>
       </c>
       <c r="D166" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="E166" t="s">
         <v>14</v>
@@ -6972,9 +6973,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B167" t="s">
         <v>28</v>
@@ -6983,7 +6984,7 @@
         <v>29</v>
       </c>
       <c r="D167" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E167" t="s">
         <v>14</v>
@@ -7004,24 +7005,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B168" t="s">
         <v>28</v>
       </c>
       <c r="C168" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="D168" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="E168" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F168" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G168" t="s">
         <v>13</v>
@@ -7036,7 +7037,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>91</v>
       </c>
@@ -7047,7 +7048,7 @@
         <v>69</v>
       </c>
       <c r="D169" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E169" t="s">
         <v>23</v>
@@ -7068,9 +7069,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B170" t="s">
         <v>28</v>
@@ -7079,13 +7080,13 @@
         <v>69</v>
       </c>
       <c r="D170" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="E170" t="s">
         <v>23</v>
       </c>
       <c r="F170" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G170" t="s">
         <v>13</v>
@@ -7100,9 +7101,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B171" t="s">
         <v>28</v>
@@ -7132,9 +7133,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B172" t="s">
         <v>28</v>
@@ -7143,28 +7144,28 @@
         <v>69</v>
       </c>
       <c r="D172" t="s">
-        <v>163</v>
+        <v>70</v>
       </c>
       <c r="E172" t="s">
         <v>23</v>
       </c>
       <c r="F172" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G172" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H172" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="I172" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J172" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>10</v>
       </c>
@@ -7175,13 +7176,13 @@
         <v>69</v>
       </c>
       <c r="D173" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E173" t="s">
         <v>23</v>
       </c>
       <c r="F173" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G173" t="s">
         <v>20</v>
@@ -7193,12 +7194,12 @@
         <v>23</v>
       </c>
       <c r="J173" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B174" t="s">
         <v>28</v>
@@ -7228,9 +7229,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B175" t="s">
         <v>28</v>
@@ -7239,13 +7240,13 @@
         <v>69</v>
       </c>
       <c r="D175" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E175" t="s">
         <v>23</v>
       </c>
       <c r="F175" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G175" t="s">
         <v>20</v>
@@ -7257,12 +7258,12 @@
         <v>23</v>
       </c>
       <c r="J175" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B176" t="s">
         <v>28</v>
@@ -7292,9 +7293,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B177" t="s">
         <v>28</v>
@@ -7303,13 +7304,13 @@
         <v>69</v>
       </c>
       <c r="D177" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E177" t="s">
         <v>23</v>
       </c>
       <c r="F177" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G177" t="s">
         <v>20</v>
@@ -7321,12 +7322,12 @@
         <v>23</v>
       </c>
       <c r="J177" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B178" t="s">
         <v>28</v>
@@ -7356,7 +7357,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>91</v>
       </c>
@@ -7367,30 +7368,30 @@
         <v>69</v>
       </c>
       <c r="D179" t="s">
-        <v>94</v>
+        <v>166</v>
       </c>
       <c r="E179" t="s">
         <v>23</v>
       </c>
       <c r="F179" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G179" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H179" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="I179" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J179" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="180" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B180" t="s">
         <v>28</v>
@@ -7399,71 +7400,71 @@
         <v>69</v>
       </c>
       <c r="D180" t="s">
+        <v>94</v>
+      </c>
+      <c r="E180" t="s">
+        <v>23</v>
+      </c>
+      <c r="F180" t="s">
+        <v>22</v>
+      </c>
+      <c r="G180" t="s">
+        <v>13</v>
+      </c>
+      <c r="H180" t="s">
+        <v>13</v>
+      </c>
+      <c r="I180" t="s">
+        <v>13</v>
+      </c>
+      <c r="J180" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>10</v>
+      </c>
+      <c r="B181" t="s">
+        <v>28</v>
+      </c>
+      <c r="C181" t="s">
+        <v>69</v>
+      </c>
+      <c r="D181" t="s">
         <v>167</v>
       </c>
-      <c r="E180" t="s">
-        <v>23</v>
-      </c>
-      <c r="F180" t="s">
+      <c r="E181" t="s">
+        <v>23</v>
+      </c>
+      <c r="F181" t="s">
         <v>15</v>
       </c>
-      <c r="G180" t="s">
-        <v>13</v>
-      </c>
-      <c r="H180" t="s">
-        <v>13</v>
-      </c>
-      <c r="I180" t="s">
-        <v>13</v>
-      </c>
-      <c r="J180" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="181" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A181" s="3" t="s">
+      <c r="G181" t="s">
+        <v>13</v>
+      </c>
+      <c r="H181" t="s">
+        <v>13</v>
+      </c>
+      <c r="I181" t="s">
+        <v>13</v>
+      </c>
+      <c r="J181" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A182" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C181" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D181" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E181" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F181" t="s">
-        <v>22</v>
-      </c>
-      <c r="G181" t="s">
-        <v>13</v>
-      </c>
-      <c r="H181" t="s">
-        <v>13</v>
-      </c>
-      <c r="I181" t="s">
-        <v>13</v>
-      </c>
-      <c r="J181" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="182" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A182" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>23</v>
@@ -7471,20 +7472,20 @@
       <c r="F182" t="s">
         <v>22</v>
       </c>
-      <c r="G182" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H182" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I182" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J182" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="183" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G182" t="s">
+        <v>13</v>
+      </c>
+      <c r="H182" t="s">
+        <v>13</v>
+      </c>
+      <c r="I182" t="s">
+        <v>13</v>
+      </c>
+      <c r="J182" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="3" t="s">
         <v>10</v>
       </c>
@@ -7495,7 +7496,7 @@
         <v>71</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>168</v>
+        <v>98</v>
       </c>
       <c r="E183" s="3" t="s">
         <v>23</v>
@@ -7516,9 +7517,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="184" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="3" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B184" s="3" t="s">
         <v>28</v>
@@ -7527,30 +7528,30 @@
         <v>71</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>72</v>
+        <v>168</v>
       </c>
       <c r="E184" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F184" s="3" t="s">
-        <v>50</v>
+      <c r="F184" t="s">
+        <v>22</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H184" s="3" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="I184" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J184" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="185" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="3" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>28</v>
@@ -7580,9 +7581,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="186" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>28</v>
@@ -7612,9 +7613,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="187" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" s="3" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>28</v>
@@ -7623,13 +7624,13 @@
         <v>71</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F187" t="s">
-        <v>22</v>
+      <c r="F187" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="G187" s="3" t="s">
         <v>20</v>
@@ -7644,9 +7645,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="188" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" s="3" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B188" s="3" t="s">
         <v>28</v>
@@ -7676,9 +7677,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="189" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>28</v>
@@ -7708,23 +7709,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" s="3" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>210</v>
+        <v>73</v>
       </c>
       <c r="E190" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F190" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F190" t="s">
         <v>22</v>
       </c>
       <c r="G190" s="3" t="s">
@@ -7740,23 +7741,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A191" t="s">
-        <v>10</v>
-      </c>
-      <c r="B191" t="s">
+    <row r="191" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A191" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B191" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C191" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="E191" t="s">
-        <v>19</v>
-      </c>
-      <c r="F191" t="s">
+      <c r="E191" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F191" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G191" s="3" t="s">
@@ -7772,7 +7773,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>10</v>
       </c>
@@ -7782,8 +7783,8 @@
       <c r="C192" t="s">
         <v>74</v>
       </c>
-      <c r="D192" t="s">
-        <v>169</v>
+      <c r="D192" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="E192" t="s">
         <v>19</v>
@@ -7804,41 +7805,41 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B193" t="s">
         <v>28</v>
       </c>
       <c r="C193" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D193" t="s">
-        <v>76</v>
+        <v>169</v>
       </c>
       <c r="E193" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F193" t="s">
-        <v>15</v>
-      </c>
-      <c r="G193" t="s">
-        <v>13</v>
-      </c>
-      <c r="H193" t="s">
-        <v>13</v>
-      </c>
-      <c r="I193" t="s">
-        <v>13</v>
-      </c>
-      <c r="J193" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="G193" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H193" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I193" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J193" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B194" t="s">
         <v>28</v>
@@ -7868,9 +7869,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B195" t="s">
         <v>28</v>
@@ -7879,7 +7880,7 @@
         <v>75</v>
       </c>
       <c r="D195" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E195" t="s">
         <v>14</v>
@@ -7900,9 +7901,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B196" t="s">
         <v>28</v>
@@ -7932,7 +7933,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>10</v>
       </c>
@@ -7943,7 +7944,7 @@
         <v>75</v>
       </c>
       <c r="D197" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="E197" t="s">
         <v>14</v>
@@ -7964,7 +7965,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>10</v>
       </c>
@@ -7975,7 +7976,7 @@
         <v>75</v>
       </c>
       <c r="D198" t="s">
-        <v>170</v>
+        <v>107</v>
       </c>
       <c r="E198" t="s">
         <v>14</v>
@@ -7996,9 +7997,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B199" t="s">
         <v>28</v>
@@ -8007,13 +8008,13 @@
         <v>75</v>
       </c>
       <c r="D199" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E199" t="s">
         <v>14</v>
       </c>
       <c r="F199" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G199" t="s">
         <v>13</v>
@@ -8028,9 +8029,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B200" t="s">
         <v>28</v>
@@ -8060,41 +8061,41 @@
         <v>13</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
+        <v>10</v>
+      </c>
+      <c r="B201" t="s">
+        <v>28</v>
+      </c>
+      <c r="C201" t="s">
+        <v>75</v>
+      </c>
+      <c r="D201" t="s">
+        <v>171</v>
+      </c>
+      <c r="E201" t="s">
+        <v>14</v>
+      </c>
+      <c r="F201" t="s">
+        <v>50</v>
+      </c>
+      <c r="G201" t="s">
+        <v>13</v>
+      </c>
+      <c r="H201" t="s">
+        <v>13</v>
+      </c>
+      <c r="I201" t="s">
+        <v>13</v>
+      </c>
+      <c r="J201" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
         <v>16</v>
-      </c>
-      <c r="B201" t="s">
-        <v>78</v>
-      </c>
-      <c r="C201" t="s">
-        <v>108</v>
-      </c>
-      <c r="D201" t="s">
-        <v>61</v>
-      </c>
-      <c r="E201" t="s">
-        <v>19</v>
-      </c>
-      <c r="F201" t="s">
-        <v>22</v>
-      </c>
-      <c r="G201" t="s">
-        <v>13</v>
-      </c>
-      <c r="H201" t="s">
-        <v>13</v>
-      </c>
-      <c r="I201" t="s">
-        <v>13</v>
-      </c>
-      <c r="J201" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A202" t="s">
-        <v>91</v>
       </c>
       <c r="B202" t="s">
         <v>78</v>
@@ -8124,9 +8125,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B203" t="s">
         <v>78</v>
@@ -8135,7 +8136,7 @@
         <v>108</v>
       </c>
       <c r="D203" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="E203" t="s">
         <v>19</v>
@@ -8156,9 +8157,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B204" t="s">
         <v>78</v>
@@ -8188,9 +8189,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B205" t="s">
         <v>78</v>
@@ -8199,7 +8200,7 @@
         <v>108</v>
       </c>
       <c r="D205" t="s">
-        <v>172</v>
+        <v>80</v>
       </c>
       <c r="E205" t="s">
         <v>19</v>
@@ -8220,9 +8221,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B206" t="s">
         <v>78</v>
@@ -8252,9 +8253,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B207" t="s">
         <v>78</v>
@@ -8284,9 +8285,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B208" t="s">
         <v>78</v>
@@ -8295,7 +8296,7 @@
         <v>108</v>
       </c>
       <c r="D208" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="E208" t="s">
         <v>19</v>
@@ -8316,9 +8317,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B209" t="s">
         <v>78</v>
@@ -8348,9 +8349,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B210" t="s">
         <v>78</v>
@@ -8380,24 +8381,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B211" t="s">
         <v>78</v>
       </c>
       <c r="C211" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="D211" t="s">
-        <v>79</v>
+        <v>211</v>
       </c>
       <c r="E211" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F211" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G211" t="s">
         <v>13</v>
@@ -8412,9 +8413,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B212" t="s">
         <v>78</v>
@@ -8444,9 +8445,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B213" t="s">
         <v>78</v>
@@ -8455,7 +8456,7 @@
         <v>82</v>
       </c>
       <c r="D213" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="E213" t="s">
         <v>23</v>
@@ -8476,9 +8477,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B214" t="s">
         <v>78</v>
@@ -8508,9 +8509,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B215" t="s">
         <v>78</v>
@@ -8540,9 +8541,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B216" t="s">
         <v>78</v>
@@ -8551,7 +8552,7 @@
         <v>82</v>
       </c>
       <c r="D216" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="E216" t="s">
         <v>23</v>
@@ -8572,9 +8573,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B217" t="s">
         <v>78</v>
@@ -8604,9 +8605,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B218" t="s">
         <v>78</v>
@@ -8615,13 +8616,13 @@
         <v>82</v>
       </c>
       <c r="D218" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
       <c r="E218" t="s">
         <v>23</v>
       </c>
       <c r="F218" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G218" t="s">
         <v>13</v>
@@ -8636,7 +8637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>10</v>
       </c>
@@ -8647,13 +8648,13 @@
         <v>82</v>
       </c>
       <c r="D219" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E219" t="s">
         <v>23</v>
       </c>
       <c r="F219" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G219" t="s">
         <v>13</v>
@@ -8668,9 +8669,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B220" t="s">
         <v>78</v>
@@ -8700,9 +8701,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B221" t="s">
         <v>78</v>
@@ -8732,18 +8733,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B222" t="s">
         <v>78</v>
       </c>
       <c r="C222" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D222" t="s">
-        <v>84</v>
+        <v>174</v>
       </c>
       <c r="E222" t="s">
         <v>23</v>
@@ -8764,9 +8765,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B223" t="s">
         <v>78</v>
@@ -8796,9 +8797,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B224" t="s">
         <v>78</v>
@@ -8828,9 +8829,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B225" t="s">
         <v>78</v>
@@ -8839,13 +8840,13 @@
         <v>83</v>
       </c>
       <c r="D225" t="s">
-        <v>175</v>
+        <v>84</v>
       </c>
       <c r="E225" t="s">
         <v>23</v>
       </c>
       <c r="F225" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G225" t="s">
         <v>13</v>
@@ -8860,7 +8861,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>10</v>
       </c>
@@ -8871,13 +8872,13 @@
         <v>83</v>
       </c>
       <c r="D226" t="s">
-        <v>85</v>
+        <v>175</v>
       </c>
       <c r="E226" t="s">
         <v>23</v>
       </c>
       <c r="F226" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G226" t="s">
         <v>13</v>
@@ -8892,9 +8893,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B227" t="s">
         <v>78</v>
@@ -8909,7 +8910,7 @@
         <v>23</v>
       </c>
       <c r="F227" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="G227" t="s">
         <v>13</v>
@@ -8924,9 +8925,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B228" t="s">
         <v>78</v>
@@ -8941,7 +8942,7 @@
         <v>23</v>
       </c>
       <c r="F228" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G228" t="s">
         <v>13</v>
@@ -8956,9 +8957,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B229" t="s">
         <v>78</v>
@@ -8967,42 +8968,42 @@
         <v>83</v>
       </c>
       <c r="D229" t="s">
+        <v>85</v>
+      </c>
+      <c r="E229" t="s">
+        <v>23</v>
+      </c>
+      <c r="F229" t="s">
+        <v>22</v>
+      </c>
+      <c r="G229" t="s">
+        <v>13</v>
+      </c>
+      <c r="H229" t="s">
+        <v>13</v>
+      </c>
+      <c r="I229" t="s">
+        <v>13</v>
+      </c>
+      <c r="J229" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
+        <v>10</v>
+      </c>
+      <c r="B230" t="s">
+        <v>78</v>
+      </c>
+      <c r="C230" t="s">
+        <v>83</v>
+      </c>
+      <c r="D230" t="s">
         <v>176</v>
       </c>
-      <c r="E229" t="s">
-        <v>23</v>
-      </c>
-      <c r="F229" t="s">
-        <v>15</v>
-      </c>
-      <c r="G229" t="s">
-        <v>13</v>
-      </c>
-      <c r="H229" t="s">
-        <v>13</v>
-      </c>
-      <c r="I229" t="s">
-        <v>13</v>
-      </c>
-      <c r="J229" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A230" t="s">
-        <v>10</v>
-      </c>
-      <c r="B230" t="s">
-        <v>86</v>
-      </c>
-      <c r="C230" t="s">
-        <v>87</v>
-      </c>
-      <c r="D230" t="s">
-        <v>88</v>
-      </c>
       <c r="E230" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F230" t="s">
         <v>15</v>
@@ -9020,7 +9021,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>10</v>
       </c>
@@ -9031,7 +9032,7 @@
         <v>87</v>
       </c>
       <c r="D231" t="s">
-        <v>177</v>
+        <v>88</v>
       </c>
       <c r="E231" t="s">
         <v>14</v>
@@ -9052,9 +9053,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B232" t="s">
         <v>86</v>
@@ -9084,9 +9085,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="B233" t="s">
         <v>86</v>
@@ -9116,24 +9117,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B234" t="s">
         <v>86</v>
       </c>
       <c r="C234" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D234" t="s">
-        <v>128</v>
+        <v>177</v>
       </c>
       <c r="E234" t="s">
         <v>14</v>
       </c>
       <c r="F234" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G234" t="s">
         <v>13</v>
@@ -9148,7 +9149,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>10</v>
       </c>
@@ -9159,13 +9160,13 @@
         <v>89</v>
       </c>
       <c r="D235" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="E235" t="s">
         <v>14</v>
       </c>
       <c r="F235" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G235" t="s">
         <v>13</v>
@@ -9180,9 +9181,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="B236" t="s">
         <v>86</v>
@@ -9212,9 +9213,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B237" t="s">
         <v>86</v>
@@ -9223,7 +9224,7 @@
         <v>89</v>
       </c>
       <c r="D237" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E237" t="s">
         <v>14</v>
@@ -9244,7 +9245,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>10</v>
       </c>
@@ -9255,7 +9256,7 @@
         <v>89</v>
       </c>
       <c r="D238" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E238" t="s">
         <v>14</v>
@@ -9276,7 +9277,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>10</v>
       </c>
@@ -9284,10 +9285,10 @@
         <v>86</v>
       </c>
       <c r="C239" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D239" t="s">
-        <v>178</v>
+        <v>85</v>
       </c>
       <c r="E239" t="s">
         <v>14</v>
@@ -9308,9 +9309,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B240" t="s">
         <v>86</v>
@@ -9340,7 +9341,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>16</v>
       </c>
@@ -9348,10 +9349,10 @@
         <v>86</v>
       </c>
       <c r="C241" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D241" t="s">
-        <v>82</v>
+        <v>178</v>
       </c>
       <c r="E241" t="s">
         <v>14</v>
@@ -9372,7 +9373,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>16</v>
       </c>
@@ -9383,7 +9384,7 @@
         <v>89</v>
       </c>
       <c r="D242" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E242" t="s">
         <v>14</v>
@@ -9404,7 +9405,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>16</v>
       </c>
@@ -9415,13 +9416,13 @@
         <v>89</v>
       </c>
       <c r="D243" t="s">
-        <v>192</v>
+        <v>84</v>
       </c>
       <c r="E243" t="s">
         <v>14</v>
       </c>
       <c r="F243" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G243" t="s">
         <v>13</v>
@@ -9436,24 +9437,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>16</v>
       </c>
       <c r="B244" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="C244" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="D244" t="s">
-        <v>65</v>
+        <v>192</v>
       </c>
       <c r="E244" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F244" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G244" t="s">
         <v>13</v>
@@ -9479,13 +9480,13 @@
         <v>63</v>
       </c>
       <c r="D245" t="s">
-        <v>195</v>
+        <v>65</v>
       </c>
       <c r="E245" t="s">
         <v>23</v>
       </c>
       <c r="F245" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G245" t="s">
         <v>13</v>
@@ -9502,71 +9503,71 @@
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
+        <v>16</v>
+      </c>
+      <c r="B246" t="s">
+        <v>20</v>
+      </c>
+      <c r="C246" t="s">
+        <v>63</v>
+      </c>
+      <c r="D246" t="s">
+        <v>195</v>
+      </c>
+      <c r="E246" t="s">
+        <v>23</v>
+      </c>
+      <c r="F246" t="s">
+        <v>22</v>
+      </c>
+      <c r="G246" t="s">
+        <v>13</v>
+      </c>
+      <c r="H246" t="s">
+        <v>13</v>
+      </c>
+      <c r="I246" t="s">
+        <v>13</v>
+      </c>
+      <c r="J246" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A247" t="s">
         <v>91</v>
       </c>
-      <c r="B246" t="s">
+      <c r="B247" t="s">
         <v>26</v>
       </c>
-      <c r="C246" s="2" t="s">
+      <c r="C247" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D246" t="s">
+      <c r="D247" t="s">
         <v>197</v>
       </c>
-      <c r="E246" t="s">
-        <v>19</v>
-      </c>
-      <c r="F246" t="s">
-        <v>22</v>
-      </c>
-      <c r="G246" t="s">
-        <v>13</v>
-      </c>
-      <c r="H246" t="s">
-        <v>13</v>
-      </c>
-      <c r="I246" t="s">
-        <v>13</v>
-      </c>
-      <c r="J246" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A247" t="s">
+      <c r="E247" t="s">
+        <v>19</v>
+      </c>
+      <c r="F247" t="s">
+        <v>22</v>
+      </c>
+      <c r="G247" t="s">
+        <v>13</v>
+      </c>
+      <c r="H247" t="s">
+        <v>13</v>
+      </c>
+      <c r="I247" t="s">
+        <v>13</v>
+      </c>
+      <c r="J247" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A248" t="s">
         <v>16</v>
-      </c>
-      <c r="B247" t="s">
-        <v>56</v>
-      </c>
-      <c r="C247" t="s">
-        <v>201</v>
-      </c>
-      <c r="D247" t="s">
-        <v>212</v>
-      </c>
-      <c r="E247" t="s">
-        <v>14</v>
-      </c>
-      <c r="F247" t="s">
-        <v>15</v>
-      </c>
-      <c r="G247" t="s">
-        <v>13</v>
-      </c>
-      <c r="H247" t="s">
-        <v>13</v>
-      </c>
-      <c r="I247" t="s">
-        <v>13</v>
-      </c>
-      <c r="J247" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A248" t="s">
-        <v>91</v>
       </c>
       <c r="B248" t="s">
         <v>56</v>
@@ -9596,9 +9597,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B249" t="s">
         <v>56</v>
@@ -9628,41 +9629,41 @@
         <v>13</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A250" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B250" s="3" t="s">
+    <row r="250" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A250" t="s">
+        <v>10</v>
+      </c>
+      <c r="B250" t="s">
         <v>56</v>
       </c>
       <c r="C250" t="s">
         <v>201</v>
       </c>
       <c r="D250" t="s">
-        <v>213</v>
-      </c>
-      <c r="E250" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E250" t="s">
         <v>14</v>
       </c>
-      <c r="F250" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G250" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H250" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I250" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J250" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A251" t="s">
-        <v>16</v>
+      <c r="F250" t="s">
+        <v>15</v>
+      </c>
+      <c r="G250" t="s">
+        <v>13</v>
+      </c>
+      <c r="H250" t="s">
+        <v>13</v>
+      </c>
+      <c r="I250" t="s">
+        <v>13</v>
+      </c>
+      <c r="J250" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A251" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="B251" s="3" t="s">
         <v>56</v>
@@ -9692,9 +9693,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B252" s="3" t="s">
         <v>56</v>
@@ -9724,35 +9725,35 @@
         <v>13</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>10</v>
       </c>
-      <c r="B253" t="s">
-        <v>20</v>
+      <c r="B253" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C253" t="s">
-        <v>63</v>
+        <v>201</v>
       </c>
       <c r="D253" t="s">
-        <v>195</v>
-      </c>
-      <c r="E253" t="s">
-        <v>23</v>
-      </c>
-      <c r="F253" t="s">
-        <v>22</v>
-      </c>
-      <c r="G253" t="s">
-        <v>13</v>
-      </c>
-      <c r="H253" t="s">
-        <v>13</v>
-      </c>
-      <c r="I253" t="s">
-        <v>13</v>
-      </c>
-      <c r="J253" t="s">
+        <v>213</v>
+      </c>
+      <c r="E253" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F253" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G253" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H253" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I253" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J253" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -9761,16 +9762,16 @@
         <v>10</v>
       </c>
       <c r="B254" t="s">
-        <v>26</v>
-      </c>
-      <c r="C254" s="2" t="s">
-        <v>55</v>
+        <v>20</v>
+      </c>
+      <c r="C254" t="s">
+        <v>63</v>
       </c>
       <c r="D254" t="s">
-        <v>47</v>
+        <v>195</v>
       </c>
       <c r="E254" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F254" t="s">
         <v>22</v>
@@ -9788,88 +9789,88 @@
         <v>13</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>10</v>
       </c>
       <c r="B255" t="s">
         <v>26</v>
       </c>
-      <c r="C255" t="s">
+      <c r="C255" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D255" t="s">
+        <v>47</v>
+      </c>
+      <c r="E255" t="s">
+        <v>19</v>
+      </c>
+      <c r="F255" t="s">
+        <v>22</v>
+      </c>
+      <c r="G255" t="s">
+        <v>13</v>
+      </c>
+      <c r="H255" t="s">
+        <v>13</v>
+      </c>
+      <c r="I255" t="s">
+        <v>13</v>
+      </c>
+      <c r="J255" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
+        <v>10</v>
+      </c>
+      <c r="B256" t="s">
+        <v>26</v>
+      </c>
+      <c r="C256" t="s">
         <v>30</v>
       </c>
-      <c r="D255" t="s">
+      <c r="D256" t="s">
         <v>124</v>
       </c>
-      <c r="E255" t="s">
-        <v>19</v>
-      </c>
-      <c r="F255" t="s">
-        <v>22</v>
-      </c>
-      <c r="G255" t="s">
-        <v>13</v>
-      </c>
-      <c r="H255" t="s">
-        <v>13</v>
-      </c>
-      <c r="I255" t="s">
-        <v>13</v>
-      </c>
-      <c r="J255" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A256" s="3" t="s">
+      <c r="E256" t="s">
+        <v>19</v>
+      </c>
+      <c r="F256" t="s">
+        <v>22</v>
+      </c>
+      <c r="G256" t="s">
+        <v>13</v>
+      </c>
+      <c r="H256" t="s">
+        <v>13</v>
+      </c>
+      <c r="I256" t="s">
+        <v>13</v>
+      </c>
+      <c r="J256" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A257" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B256" t="s">
+      <c r="B257" t="s">
         <v>28</v>
       </c>
-      <c r="C256" t="s">
+      <c r="C257" t="s">
         <v>75</v>
       </c>
-      <c r="D256" t="s">
+      <c r="D257" t="s">
         <v>170</v>
       </c>
-      <c r="E256" t="s">
+      <c r="E257" t="s">
         <v>14</v>
       </c>
-      <c r="F256" t="s">
+      <c r="F257" t="s">
         <v>15</v>
-      </c>
-      <c r="G256" t="s">
-        <v>13</v>
-      </c>
-      <c r="H256" t="s">
-        <v>13</v>
-      </c>
-      <c r="I256" t="s">
-        <v>13</v>
-      </c>
-      <c r="J256" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A257" t="s">
-        <v>91</v>
-      </c>
-      <c r="B257" t="s">
-        <v>20</v>
-      </c>
-      <c r="C257" t="s">
-        <v>63</v>
-      </c>
-      <c r="D257" t="s">
-        <v>149</v>
-      </c>
-      <c r="E257" t="s">
-        <v>23</v>
-      </c>
-      <c r="F257" t="s">
-        <v>50</v>
       </c>
       <c r="G257" t="s">
         <v>13</v>
@@ -9886,66 +9887,66 @@
     </row>
     <row r="258" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B258" t="s">
+        <v>20</v>
+      </c>
+      <c r="C258" t="s">
+        <v>63</v>
+      </c>
+      <c r="D258" t="s">
+        <v>149</v>
+      </c>
+      <c r="E258" t="s">
+        <v>23</v>
+      </c>
+      <c r="F258" t="s">
+        <v>50</v>
+      </c>
+      <c r="G258" t="s">
+        <v>13</v>
+      </c>
+      <c r="H258" t="s">
+        <v>13</v>
+      </c>
+      <c r="I258" t="s">
+        <v>13</v>
+      </c>
+      <c r="J258" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
+        <v>10</v>
+      </c>
+      <c r="B259" t="s">
         <v>26</v>
       </c>
-      <c r="C258" t="s">
+      <c r="C259" t="s">
         <v>27</v>
       </c>
-      <c r="D258" t="s">
+      <c r="D259" t="s">
         <v>120</v>
       </c>
-      <c r="E258" t="s">
+      <c r="E259" t="s">
         <v>14</v>
       </c>
-      <c r="F258" t="s">
+      <c r="F259" t="s">
         <v>15</v>
       </c>
-      <c r="G258" t="s">
+      <c r="G259" t="s">
         <v>28</v>
       </c>
-      <c r="H258" t="s">
+      <c r="H259" t="s">
         <v>29</v>
       </c>
-      <c r="I258" t="s">
+      <c r="I259" t="s">
         <v>14</v>
       </c>
-      <c r="J258" t="s">
+      <c r="J259" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A259" t="s">
-        <v>91</v>
-      </c>
-      <c r="B259" t="s">
-        <v>20</v>
-      </c>
-      <c r="C259" t="s">
-        <v>60</v>
-      </c>
-      <c r="D259" t="s">
-        <v>199</v>
-      </c>
-      <c r="E259" t="s">
-        <v>23</v>
-      </c>
-      <c r="F259" t="s">
-        <v>22</v>
-      </c>
-      <c r="G259" t="s">
-        <v>13</v>
-      </c>
-      <c r="H259" t="s">
-        <v>13</v>
-      </c>
-      <c r="I259" t="s">
-        <v>13</v>
-      </c>
-      <c r="J259" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.35">
@@ -9959,25 +9960,25 @@
         <v>60</v>
       </c>
       <c r="D260" t="s">
-        <v>92</v>
+        <v>199</v>
       </c>
       <c r="E260" t="s">
         <v>23</v>
       </c>
       <c r="F260" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G260" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H260" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I260" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J260" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.35">
@@ -9985,41 +9986,78 @@
         <v>91</v>
       </c>
       <c r="B261" t="s">
+        <v>20</v>
+      </c>
+      <c r="C261" t="s">
+        <v>60</v>
+      </c>
+      <c r="D261" t="s">
+        <v>92</v>
+      </c>
+      <c r="E261" t="s">
+        <v>23</v>
+      </c>
+      <c r="F261" t="s">
+        <v>14</v>
+      </c>
+      <c r="G261" t="s">
+        <v>11</v>
+      </c>
+      <c r="H261" t="s">
+        <v>12</v>
+      </c>
+      <c r="I261" t="s">
+        <v>14</v>
+      </c>
+      <c r="J261" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A262" t="s">
+        <v>91</v>
+      </c>
+      <c r="B262" t="s">
         <v>26</v>
       </c>
-      <c r="C261" t="s">
+      <c r="C262" t="s">
         <v>30</v>
       </c>
-      <c r="D261" t="s">
+      <c r="D262" t="s">
         <v>200</v>
       </c>
-      <c r="E261" t="s">
-        <v>19</v>
-      </c>
-      <c r="F261" t="s">
-        <v>22</v>
-      </c>
-      <c r="G261" t="s">
-        <v>13</v>
-      </c>
-      <c r="H261" t="s">
-        <v>13</v>
-      </c>
-      <c r="I261" t="s">
-        <v>13</v>
-      </c>
-      <c r="J261" t="s">
+      <c r="E262" t="s">
+        <v>19</v>
+      </c>
+      <c r="F262" t="s">
+        <v>22</v>
+      </c>
+      <c r="G262" t="s">
+        <v>13</v>
+      </c>
+      <c r="H262" t="s">
+        <v>13</v>
+      </c>
+      <c r="I262" t="s">
+        <v>13</v>
+      </c>
+      <c r="J262" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J261" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:J258">
-      <sortCondition ref="D1:D260"/>
+  <autoFilter ref="A1:J262" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Other Soil Properties"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:J259">
+      <sortCondition ref="D1:D261"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:J253">
-    <sortCondition ref="D2:D253"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:J254">
+    <sortCondition ref="D2:D254"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>